<commit_message>
Add nearshore results to the xlsx
</commit_message>
<xml_diff>
--- a/results/Total_Results.xlsx
+++ b/results/Total_Results.xlsx
@@ -1,24 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lkilcher/Dropbox/work/mhk/wave_res/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{691C9974-35BB-B444-8272-4B97601E5B8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57EDE7B-35E9-5D41-B918-D36992C96934}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29680" yWindow="-3140" windowWidth="24640" windowHeight="14000" activeTab="5"/>
+    <workbookView xWindow="-29680" yWindow="-3140" windowWidth="24640" windowHeight="14000" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Baseline" sheetId="2" r:id="rId1"/>
-    <sheet name="Extraction" sheetId="1" r:id="rId2"/>
-    <sheet name="EPRI2011" sheetId="4" r:id="rId3"/>
-    <sheet name="Summary" sheetId="3" r:id="rId4"/>
-    <sheet name="COMPARE" sheetId="5" r:id="rId5"/>
-    <sheet name="one-way" sheetId="6" r:id="rId6"/>
+    <sheet name="EEZ.bl" sheetId="2" r:id="rId1"/>
+    <sheet name="EEZ.ex" sheetId="1" r:id="rId2"/>
+    <sheet name="Near.bl" sheetId="7" r:id="rId3"/>
+    <sheet name="Near.ex" sheetId="8" r:id="rId4"/>
+    <sheet name="EPRI2011" sheetId="4" r:id="rId5"/>
+    <sheet name="EEZ.Summary" sheetId="3" r:id="rId6"/>
+    <sheet name="EEZ.COMPARE" sheetId="5" r:id="rId7"/>
+    <sheet name="one-way" sheetId="6" r:id="rId8"/>
+    <sheet name="Near.Summary" sheetId="9" r:id="rId9"/>
+    <sheet name="Near.COMPARE" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -57,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="43">
   <si>
     <t>bdir</t>
   </si>
@@ -177,16 +181,21 @@
   </si>
   <si>
     <t>Offshore</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>Flux (kW/m)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -620,9 +629,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -669,54 +677,53 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="44">
-    <cellStyle name="20% - Accent1" xfId="21" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="25" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="29" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="33" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="37" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="41" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="22" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="26" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="30" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="34" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="38" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="42" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="23" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="27" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="31" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="35" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="39" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="43" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="24" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="28" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="32" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="36" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="40" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="9" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="13" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="15" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Explanatory Text" xfId="18" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="8" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="4" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="5" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="6" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="7" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="11" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="14" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="10" builtinId="28" customBuiltin="1"/>
+  <cellStyles count="43">
+    <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="24" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="32" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="36" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="40" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="21" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="25" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="29" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="33" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="37" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="41" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="26" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="30" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="34" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="38" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="42" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="23" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="27" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="31" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="35" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="39" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="8" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="12" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="14" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="17" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="7" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="3" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="5" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="6" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="10" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="17" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="12" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
-    <cellStyle name="Title" xfId="3" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="19" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="16" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="16" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1027,342 +1034,390 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="B1" sqref="B1:N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
       <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
+        <v>1994474</v>
+      </c>
+      <c r="C2">
         <v>415.51956492288002</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2">
         <v>60.435628523519902</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2">
         <v>475.95519344640002</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2">
         <v>355.08397228031998</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2">
         <v>753.70511204351999</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2">
+        <v>815923068928</v>
+      </c>
+      <c r="I2">
         <v>-3.5707919339999998E-2</v>
       </c>
-      <c r="H2" s="2">
-        <v>-463.56144340992</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2">
-        <v>684.12123807744001</v>
-      </c>
-      <c r="K2" s="2">
-        <v>-134.31024635904001</v>
-      </c>
-      <c r="L2" s="2">
-        <v>86.213864693760002</v>
-      </c>
-      <c r="M2" s="3">
-        <f>C2/L2</f>
-        <v>0.70099662900153137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>-485.87193729024</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>715.17061152767997</v>
+      </c>
+      <c r="M2">
+        <v>-141.13397071872001</v>
+      </c>
+      <c r="N2">
+        <v>88.12901093376</v>
+      </c>
+      <c r="O2" s="2">
+        <f>D2/N2</f>
+        <v>0.68576315430278523</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
+        <v>1908679.5</v>
+      </c>
+      <c r="C3">
         <v>106.11181252608</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3">
         <v>105.85829560320001</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3">
         <v>211.97010812927999</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3">
         <v>0.25350921407999999</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3">
         <v>347.68104849408002</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3">
+        <v>890959429632</v>
+      </c>
+      <c r="I3">
         <v>-3.9526883212800001</v>
       </c>
-      <c r="H3" s="2">
-        <v>-794.47126474751997</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2">
-        <v>1162.4254862131199</v>
-      </c>
-      <c r="K3" s="2">
-        <v>-194.07164473344</v>
-      </c>
-      <c r="L3" s="2">
-        <v>169.92994811904001</v>
-      </c>
-      <c r="M3" s="3">
-        <f t="shared" ref="M3:M8" si="0">C3/L3</f>
-        <v>0.62295255647958958</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>-832.66137980927999</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>1217.2810872422399</v>
+      </c>
+      <c r="M3">
+        <v>-203.64626362368</v>
+      </c>
+      <c r="N3">
+        <v>177.02070755328</v>
+      </c>
+      <c r="O3" s="2">
+        <f t="shared" ref="O3:O8" si="0">D3/N3</f>
+        <v>0.59799950563037141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
+        <v>4354267</v>
+      </c>
+      <c r="C4">
         <v>367.62121027583999</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4">
         <v>288.08646967295903</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4">
         <v>655.70767994879998</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4">
         <v>79.534812364800004</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4">
         <v>1159.13807265792</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4">
+        <v>895672909824</v>
+      </c>
+      <c r="I4" s="3">
         <v>-8.9609735625000004E-5</v>
       </c>
-      <c r="H4" s="2">
-        <v>-180.11052466176</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0</v>
-      </c>
-      <c r="J4" s="2">
-        <v>253.44157286399999</v>
-      </c>
-      <c r="K4" s="2">
-        <v>-65.774450749440007</v>
-      </c>
-      <c r="L4" s="2">
-        <v>7.5565542835199997</v>
-      </c>
-      <c r="M4" s="3">
+      <c r="J4">
+        <v>-193.18612058112001</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>271.20508796927999</v>
+      </c>
+      <c r="M4">
+        <v>-70.596739645439996</v>
+      </c>
+      <c r="N4">
+        <v>7.4222081203199997</v>
+      </c>
+      <c r="O4" s="2">
         <f t="shared" si="0"/>
-        <v>38.124052162404688</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+        <v>38.814119060371823</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
+        <v>5543553</v>
+      </c>
+      <c r="C5">
         <v>1038.6419869286401</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5">
         <v>609.38988158975906</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5">
         <v>1648.0318685184</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5">
         <v>429.25232062463999</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5">
         <v>2863.7153918976001</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5">
+        <v>3208809021440</v>
+      </c>
+      <c r="I5">
         <v>-11.19832539648</v>
       </c>
-      <c r="H5" s="2">
-        <v>-4447.9501959168001</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2">
-        <v>6544.1922337996803</v>
-      </c>
-      <c r="K5" s="2">
-        <v>-1127.13498329088</v>
-      </c>
-      <c r="L5" s="2">
-        <v>957.91434792960001</v>
-      </c>
-      <c r="M5" s="3">
+      <c r="J5">
+        <v>-4634.0587074355199</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>6806.8500465254401</v>
+      </c>
+      <c r="M5">
+        <v>-1175.7644483788799</v>
+      </c>
+      <c r="N5">
+        <v>985.83310761984001</v>
+      </c>
+      <c r="O5" s="2">
         <f t="shared" si="0"/>
-        <v>0.63616322576947659</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0.61814710510285875</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
+        <v>914020.3125</v>
+      </c>
+      <c r="C6">
         <v>12.862077296640001</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6">
         <v>14.826799810559899</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6">
         <v>27.6888771072</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6">
         <v>-1.9647246163200001</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6">
         <v>43.718509854719997</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6">
+        <v>693228273664</v>
+      </c>
+      <c r="I6">
         <v>-0.95244830975999994</v>
       </c>
-      <c r="H6" s="2">
-        <v>-236.56279252991999</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2">
-        <v>362.22252515328</v>
-      </c>
-      <c r="K6" s="2">
-        <v>-69.333101936640006</v>
-      </c>
-      <c r="L6" s="2">
-        <v>55.374224424959998</v>
-      </c>
-      <c r="M6" s="3">
+      <c r="J6">
+        <v>-238.85829488639999</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>365.64395409408002</v>
+      </c>
+      <c r="M6">
+        <v>-70.060857507839998</v>
+      </c>
+      <c r="N6">
+        <v>55.772390952960002</v>
+      </c>
+      <c r="O6" s="2">
         <f t="shared" si="0"/>
-        <v>0.26775634267622722</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0.26584479448021581</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
+        <v>102083.265625</v>
+      </c>
+      <c r="C7">
         <v>5.7789935846400002</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D7">
         <v>1.72249800192</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7">
         <v>7.5014915865600003</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7">
         <v>4.0564947417599999</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7">
         <v>12.731744194559999</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7">
+        <v>210565857280</v>
+      </c>
+      <c r="I7">
         <v>-6.4558402274999998E-3</v>
       </c>
-      <c r="H7" s="2">
-        <v>-48.639408599040003</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0</v>
-      </c>
-      <c r="J7" s="2">
-        <v>79.707247288320005</v>
-      </c>
-      <c r="K7" s="2">
-        <v>-20.3947152384</v>
-      </c>
-      <c r="L7" s="2">
-        <v>10.66665702912</v>
-      </c>
-      <c r="M7" s="3">
+      <c r="J7">
+        <v>-49.127860592639998</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>80.424462827520003</v>
+      </c>
+      <c r="M7">
+        <v>-20.579351930880001</v>
+      </c>
+      <c r="N7">
+        <v>10.710778275839999</v>
+      </c>
+      <c r="O7" s="2">
         <f t="shared" si="0"/>
-        <v>0.1614843335843251</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0.16081912607652332</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8">
+        <v>14817077</v>
+      </c>
+      <c r="C8">
         <v>1946.5356455347201</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D8">
         <v>1080.3195732019101</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8">
         <v>3026.8552187366399</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8">
         <v>866.21638460928</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8">
         <v>5180.6898791424001</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8">
+        <v>6715158298624</v>
+      </c>
+      <c r="I8">
         <v>-16.1457153968231</v>
       </c>
-      <c r="H8" s="2">
-        <v>-6171.2956298649597</v>
-      </c>
-      <c r="I8" s="2">
-        <v>0</v>
-      </c>
-      <c r="J8" s="2">
-        <v>9086.1103033958407</v>
-      </c>
-      <c r="K8" s="2">
-        <v>-1611.01914230784</v>
-      </c>
-      <c r="L8" s="2">
-        <v>1287.65559647999</v>
-      </c>
-      <c r="M8" s="3">
+      <c r="J8">
+        <v>-6433.7643005951904</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>9456.5752501862298</v>
+      </c>
+      <c r="M8">
+        <v>-1681.7816318054399</v>
+      </c>
+      <c r="N8">
+        <v>1324.8882034559999</v>
+      </c>
+      <c r="O8" s="2">
         <f t="shared" si="0"/>
-        <v>0.83898177133321539</v>
+        <v>0.81540432648118744</v>
       </c>
     </row>
   </sheetData>
@@ -1370,324 +1425,622 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L8"/>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FFF2529-D61C-C04A-AE20-738CA7021AB0}">
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>EEZ.Summary!A2</f>
+        <v>West Coast</v>
+      </c>
+      <c r="B2">
+        <f>EPRI2011!B2</f>
+        <v>590</v>
+      </c>
+      <c r="C2">
+        <f>Near.Summary!F2</f>
+        <v>410</v>
+      </c>
+      <c r="D2">
+        <f>Near.Summary!G2</f>
+        <v>410</v>
+      </c>
+      <c r="E2">
+        <f>AVERAGE(C2:D2)</f>
+        <v>410</v>
+      </c>
+      <c r="F2" s="2">
+        <f t="shared" ref="F2:F3" si="0">(E2-B2)/B2</f>
+        <v>-0.30508474576271188</v>
+      </c>
+      <c r="G2" s="2">
+        <f>(D2-E2)/B2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>EEZ.Summary!A3</f>
+        <v>East Coast</v>
+      </c>
+      <c r="B3">
+        <f>EPRI2011!B3</f>
+        <v>240</v>
+      </c>
+      <c r="C3">
+        <f>Near.Summary!F3</f>
+        <v>90</v>
+      </c>
+      <c r="D3">
+        <f>Near.Summary!G3</f>
+        <v>90</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E8" si="1">AVERAGE(C3:D3)</f>
+        <v>90</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.625</v>
+      </c>
+      <c r="G3" s="2">
+        <f t="shared" ref="G3:G8" si="2">(D3-E3)/B3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f>EEZ.Summary!A4</f>
+        <v>Hawaii</v>
+      </c>
+      <c r="B4">
+        <f>EPRI2011!B4</f>
+        <v>130</v>
+      </c>
+      <c r="C4">
+        <f>Near.Summary!F4</f>
+        <v>40</v>
+      </c>
+      <c r="D4">
+        <f>Near.Summary!G4</f>
+        <v>40</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="F4" s="2">
+        <f>(E4-B4)/B4</f>
+        <v>-0.69230769230769229</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="str">
+        <f>EEZ.Summary!A5</f>
+        <v>Alaska</v>
+      </c>
+      <c r="B5">
+        <f>EPRI2011!B5</f>
+        <v>1570</v>
+      </c>
+      <c r="C5">
+        <f>Near.Summary!F5</f>
+        <v>1190</v>
+      </c>
+      <c r="D5">
+        <f>Near.Summary!G5</f>
+        <v>1200</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>1195</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" ref="F5:F8" si="3">(E5-B5)/B5</f>
+        <v>-0.23885350318471338</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="2"/>
+        <v>3.1847133757961785E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="str">
+        <f>EEZ.Summary!A6</f>
+        <v>Gulf of Mexico</v>
+      </c>
+      <c r="B6">
+        <f>EPRI2011!B6</f>
+        <v>80</v>
+      </c>
+      <c r="C6">
+        <f>Near.Summary!F6</f>
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <f>Near.Summary!G6</f>
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="3"/>
+        <v>-0.75</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="str">
+        <f>EEZ.Summary!A7</f>
+        <v>Puerto Rico + US V.I.</v>
+      </c>
+      <c r="B7">
+        <f>EPRI2011!B7</f>
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <f>Near.Summary!F7</f>
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <f>Near.Summary!G7</f>
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="3"/>
+        <v>-0.33333333333333331</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="str">
+        <f>EEZ.Summary!A8</f>
+        <v>TOTAL</v>
+      </c>
+      <c r="B8">
+        <f>EPRI2011!B8</f>
+        <v>2640</v>
+      </c>
+      <c r="C8">
+        <f>Near.Summary!F8</f>
+        <v>1770</v>
+      </c>
+      <c r="D8">
+        <f>Near.Summary!G8</f>
+        <v>1780</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>1775</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="3"/>
+        <v>-0.32765151515151514</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="2"/>
+        <v>1.893939393939394E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:N8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="11" customWidth="1"/>
+    <col min="3" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
       <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
+        <v>1994474</v>
+      </c>
+      <c r="C2">
         <v>140.81227100160001</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2">
         <v>24.2461550591999</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2">
         <v>165.0584260608</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2">
         <v>116.5661159424</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2">
         <v>213.75726698496001</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2">
+        <v>815923068928</v>
+      </c>
+      <c r="I2">
         <v>-0.25081413000000002</v>
       </c>
-      <c r="H2" s="2">
-        <v>-638.6412601344</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2">
-        <v>996.50274164736004</v>
-      </c>
-      <c r="K2" s="2">
-        <v>-168.83148840960001</v>
-      </c>
-      <c r="L2" s="2">
-        <v>188.77920313344001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>-656.99968155648003</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>1039.4720570572799</v>
+      </c>
+      <c r="M2">
+        <v>-174.67445157888</v>
+      </c>
+      <c r="N2">
+        <v>207.54709807104001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
+        <v>1908679.5</v>
+      </c>
+      <c r="C3">
         <v>37.774595604479998</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3">
         <v>44.471633264639998</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3">
         <v>82.246228869120003</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3">
         <v>-6.6970253260800003</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3">
         <v>112.97421656064</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3">
+        <v>890959429632</v>
+      </c>
+      <c r="I3">
         <v>-26.841104209920001</v>
       </c>
-      <c r="H3" s="2">
-        <v>-838.60958183423998</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2">
-        <v>1275.76820023296</v>
-      </c>
-      <c r="K3" s="2">
-        <v>-199.84236158976</v>
-      </c>
-      <c r="L3" s="2">
-        <v>210.47496646656001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>-865.39938299903997</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>1334.8596921139199</v>
+      </c>
+      <c r="M3">
+        <v>-207.67210733568001</v>
+      </c>
+      <c r="N3">
+        <v>234.94707290112001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
+        <v>4354267</v>
+      </c>
+      <c r="C4">
         <v>105.22884489216</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4">
         <v>40.506966589439998</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4">
         <v>145.7358114816</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4">
         <v>64.721887272960004</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4">
         <v>204.98767331328</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4">
+        <v>895672909824</v>
+      </c>
+      <c r="I4">
         <v>-4.160492878125E-4</v>
       </c>
-      <c r="H4" s="2">
-        <v>-299.83843491840003</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0</v>
-      </c>
-      <c r="J4" s="2">
-        <v>493.59434514432002</v>
-      </c>
-      <c r="K4" s="2">
-        <v>-105.62902523904</v>
-      </c>
-      <c r="L4" s="2">
-        <v>88.12649029632</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>-312.09215950847999</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>526.95061315583996</v>
+      </c>
+      <c r="M4">
+        <v>-110.8722561024</v>
+      </c>
+      <c r="N4">
+        <v>103.98570418176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
+        <v>5543553</v>
+      </c>
+      <c r="C5">
         <v>338.27768942592002</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5">
         <v>192.61272489984</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5">
         <v>530.89041432576005</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5">
         <v>145.66494658560001</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5">
         <v>719.74887849983998</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5">
+        <v>3208809021440</v>
+      </c>
+      <c r="I5">
         <v>-66.731992473600002</v>
       </c>
-      <c r="H5" s="2">
-        <v>-5100.0163172352004</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2">
-        <v>7732.8532321075199</v>
-      </c>
-      <c r="K5" s="2">
-        <v>-1181.1038940364799</v>
-      </c>
-      <c r="L5" s="2">
-        <v>1385.0584468684799</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <v>-5234.0997331353601</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>8032.2743894016003</v>
+      </c>
+      <c r="M5">
+        <v>-1219.05547247616</v>
+      </c>
+      <c r="N5">
+        <v>1512.4438922035199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
+        <v>914020.3125</v>
+      </c>
+      <c r="C6">
         <v>4.2193906559999999</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6">
         <v>6.4259452339200003</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6">
         <v>10.64533588992</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6">
         <v>-2.2065554188799998</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6">
         <v>14.38372713984</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6">
+        <v>693228273664</v>
+      </c>
+      <c r="I6">
         <v>-15.975343733760001</v>
       </c>
-      <c r="H6" s="2">
-        <v>-237.60235364351999</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2">
-        <v>376.54606086144003</v>
-      </c>
-      <c r="K6" s="2">
-        <v>-67.712982405120002</v>
-      </c>
-      <c r="L6" s="2">
-        <v>55.255355289599997</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <v>-239.0395834368</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>380.04675084287999</v>
+      </c>
+      <c r="M6">
+        <v>-68.246321479680006</v>
+      </c>
+      <c r="N6">
+        <v>56.785530224639999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
+        <v>102083.265625</v>
+      </c>
+      <c r="C7">
         <v>2.4765750604800001</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D7">
         <v>0.249882574079999</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7">
         <v>2.72645763456</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7">
         <v>2.22669206592</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7">
         <v>3.6085865510400001</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7">
+        <v>210565857280</v>
+      </c>
+      <c r="I7">
         <v>-2.699095503E-2</v>
       </c>
-      <c r="H7" s="2">
-        <v>-54.344445358080002</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0</v>
-      </c>
-      <c r="J7" s="2">
-        <v>101.30367418368</v>
-      </c>
-      <c r="K7" s="2">
-        <v>-20.478178836480001</v>
-      </c>
-      <c r="L7" s="2">
-        <v>26.45405405184</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <v>-54.755322716160002</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>102.35866411008</v>
+      </c>
+      <c r="M7">
+        <v>-20.635700736</v>
+      </c>
+      <c r="N7">
+        <v>26.940646963199999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8">
+        <v>14817077</v>
+      </c>
+      <c r="C8">
         <v>628.78936664063997</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D8">
         <v>308.51330762112002</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8">
         <v>937.30267426175999</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8">
         <v>320.27606112192001</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8">
         <v>1269.4603490495999</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8">
+        <v>6715158298624</v>
+      </c>
+      <c r="I8">
         <v>-109.826661551597</v>
       </c>
-      <c r="H8" s="2">
-        <v>-7169.0523931238404</v>
-      </c>
-      <c r="I8" s="2">
-        <v>0</v>
-      </c>
-      <c r="J8" s="2">
-        <v>10976.5682541772</v>
-      </c>
-      <c r="K8" s="2">
-        <v>-1743.5979305164799</v>
-      </c>
-      <c r="L8" s="2">
-        <v>1954.1485161062401</v>
+      <c r="J8">
+        <v>-7362.3858633523196</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>11415.9621666815</v>
+      </c>
+      <c r="M8">
+        <v>-1801.1563097088001</v>
+      </c>
+      <c r="N8">
+        <v>2142.6499445452801</v>
       </c>
     </row>
   </sheetData>
@@ -1696,7 +2049,735 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51B6B5B9-50BB-3A4E-98D2-F24B327EABE8}">
+  <dimension ref="A1:N8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>2556410.5</v>
+      </c>
+      <c r="C2">
+        <v>414.89609736192</v>
+      </c>
+      <c r="D2">
+        <v>22.444796313600001</v>
+      </c>
+      <c r="E2">
+        <v>437.34089367552002</v>
+      </c>
+      <c r="F2">
+        <v>392.45133692927999</v>
+      </c>
+      <c r="G2">
+        <v>627.41410775040004</v>
+      </c>
+      <c r="H2">
+        <v>56433676288</v>
+      </c>
+      <c r="I2">
+        <v>-1.88686458E-2</v>
+      </c>
+      <c r="J2">
+        <v>-5.0460352742400003</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>7.0557412992000001</v>
+      </c>
+      <c r="M2">
+        <v>-1.6264177612799999</v>
+      </c>
+      <c r="N2">
+        <v>0.36441943391999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>3198674.25</v>
+      </c>
+      <c r="C3">
+        <v>93.129650626559993</v>
+      </c>
+      <c r="D3">
+        <v>7.4198775398399999</v>
+      </c>
+      <c r="E3">
+        <v>100.54952816639999</v>
+      </c>
+      <c r="F3">
+        <v>85.709791027199998</v>
+      </c>
+      <c r="G3">
+        <v>142.14234230784001</v>
+      </c>
+      <c r="H3">
+        <v>82097455104</v>
+      </c>
+      <c r="I3">
+        <v>-0.75569366400000004</v>
+      </c>
+      <c r="J3">
+        <v>-13.99678910976</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>23.031284060160001</v>
+      </c>
+      <c r="M3">
+        <v>-3.66329352192</v>
+      </c>
+      <c r="N3">
+        <v>4.6155111283199997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>1749916.125</v>
+      </c>
+      <c r="C4">
+        <v>37.887400857599999</v>
+      </c>
+      <c r="D4">
+        <v>117.97534513152</v>
+      </c>
+      <c r="E4">
+        <v>155.86274598911999</v>
+      </c>
+      <c r="F4">
+        <v>-80.087953244160005</v>
+      </c>
+      <c r="G4">
+        <v>261.07921195007998</v>
+      </c>
+      <c r="H4">
+        <v>31162910720</v>
+      </c>
+      <c r="I4" s="3">
+        <v>-2.7204686865234298E-5</v>
+      </c>
+      <c r="J4">
+        <v>-1.8461348198400001</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>3.0574395878399998</v>
+      </c>
+      <c r="M4">
+        <v>-0.65093177280000003</v>
+      </c>
+      <c r="N4">
+        <v>0.56034587424000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>11205635</v>
+      </c>
+      <c r="C5">
+        <v>1135.2602984447999</v>
+      </c>
+      <c r="D5">
+        <v>230.231973887999</v>
+      </c>
+      <c r="E5">
+        <v>1365.4922723328</v>
+      </c>
+      <c r="F5">
+        <v>905.02861160448003</v>
+      </c>
+      <c r="G5">
+        <v>2130.87376637952</v>
+      </c>
+      <c r="H5">
+        <v>323765665792</v>
+      </c>
+      <c r="I5">
+        <v>-0.92652361536000005</v>
+      </c>
+      <c r="J5">
+        <v>-125.89252829183999</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>213.27095439359999</v>
+      </c>
+      <c r="M5">
+        <v>-32.364706652160002</v>
+      </c>
+      <c r="N5">
+        <v>54.088896675839997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>2723843.5</v>
+      </c>
+      <c r="C6">
+        <v>24.46945572864</v>
+      </c>
+      <c r="D6">
+        <v>2.5340210380800001</v>
+      </c>
+      <c r="E6">
+        <v>27.003476766719999</v>
+      </c>
+      <c r="F6">
+        <v>21.935436933119998</v>
+      </c>
+      <c r="G6">
+        <v>38.061782323199999</v>
+      </c>
+      <c r="H6">
+        <v>64780673024</v>
+      </c>
+      <c r="I6">
+        <v>-0.17584163495999999</v>
+      </c>
+      <c r="J6">
+        <v>-5.0355451391999999</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>9.2287987584</v>
+      </c>
+      <c r="M6">
+        <v>-1.5320860166400001</v>
+      </c>
+      <c r="N6">
+        <v>2.48532721152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>636362.125</v>
+      </c>
+      <c r="C7">
+        <v>17.640082360320001</v>
+      </c>
+      <c r="D7">
+        <v>2.2209394790399899</v>
+      </c>
+      <c r="E7">
+        <v>19.861021839359999</v>
+      </c>
+      <c r="F7">
+        <v>15.41914176</v>
+      </c>
+      <c r="G7">
+        <v>31.64697532416</v>
+      </c>
+      <c r="H7">
+        <v>13952835584</v>
+      </c>
+      <c r="I7">
+        <v>-6.3061274474999996E-3</v>
+      </c>
+      <c r="J7">
+        <v>-0.62383772352</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>1.1533521120000001</v>
+      </c>
+      <c r="M7">
+        <v>-0.30683424240000001</v>
+      </c>
+      <c r="N7">
+        <v>0.21637522368000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>22070840</v>
+      </c>
+      <c r="C8">
+        <v>1723.2829853798401</v>
+      </c>
+      <c r="D8">
+        <v>382.82695339007898</v>
+      </c>
+      <c r="E8">
+        <v>2106.1099387699201</v>
+      </c>
+      <c r="F8">
+        <v>1340.4563650099201</v>
+      </c>
+      <c r="G8">
+        <v>3231.2181860351998</v>
+      </c>
+      <c r="H8">
+        <v>572193243136</v>
+      </c>
+      <c r="I8">
+        <v>-1.8832608922543601</v>
+      </c>
+      <c r="J8">
+        <v>-152.44087035839999</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>256.79757021120002</v>
+      </c>
+      <c r="M8">
+        <v>-40.144269967200003</v>
+      </c>
+      <c r="N8">
+        <v>62.330875547520002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F8BC87F-C28B-3641-A3EB-72C101404CE7}">
+  <dimension ref="A1:N8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>2556410.5</v>
+      </c>
+      <c r="C2">
+        <v>65.858717184</v>
+      </c>
+      <c r="D2">
+        <v>8.5499932262399998</v>
+      </c>
+      <c r="E2">
+        <v>74.408710410240005</v>
+      </c>
+      <c r="F2">
+        <v>57.30871947264</v>
+      </c>
+      <c r="G2">
+        <v>131.92060133376</v>
+      </c>
+      <c r="H2">
+        <v>56433676288</v>
+      </c>
+      <c r="I2">
+        <v>-0.13535362451999999</v>
+      </c>
+      <c r="J2">
+        <v>-7.3082574796799999</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>11.794930452479999</v>
+      </c>
+      <c r="M2">
+        <v>-2.3416124736000001</v>
+      </c>
+      <c r="N2">
+        <v>2.00970896832</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>3198674.25</v>
+      </c>
+      <c r="C3">
+        <v>45.21558460416</v>
+      </c>
+      <c r="D3">
+        <v>6.9685802803200003</v>
+      </c>
+      <c r="E3">
+        <v>52.184164884479998</v>
+      </c>
+      <c r="F3">
+        <v>38.247004323840002</v>
+      </c>
+      <c r="G3">
+        <v>80.880904519680001</v>
+      </c>
+      <c r="H3">
+        <v>82097455104</v>
+      </c>
+      <c r="I3">
+        <v>-5.6587548057600001</v>
+      </c>
+      <c r="J3">
+        <v>-14.891890114560001</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>24.795851366400001</v>
+      </c>
+      <c r="M3">
+        <v>-3.8179948416</v>
+      </c>
+      <c r="N3">
+        <v>0.42721191984000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>1749916.125</v>
+      </c>
+      <c r="C4">
+        <v>7.5513812582400002</v>
+      </c>
+      <c r="D4">
+        <v>17.447881512959999</v>
+      </c>
+      <c r="E4">
+        <v>24.999262771200002</v>
+      </c>
+      <c r="F4">
+        <v>-9.8965002547199994</v>
+      </c>
+      <c r="G4">
+        <v>43.753372692479999</v>
+      </c>
+      <c r="H4">
+        <v>31162910720</v>
+      </c>
+      <c r="I4">
+        <v>-1.2652651429687501E-4</v>
+      </c>
+      <c r="J4">
+        <v>-2.8499579366400001</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>5.1997554739199998</v>
+      </c>
+      <c r="M4">
+        <v>-1.17117534816</v>
+      </c>
+      <c r="N4">
+        <v>1.17849569472</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>11205635</v>
+      </c>
+      <c r="C5">
+        <v>543.93486557183996</v>
+      </c>
+      <c r="D5">
+        <v>157.38031325183999</v>
+      </c>
+      <c r="E5">
+        <v>701.31517882367996</v>
+      </c>
+      <c r="F5">
+        <v>386.55455232000003</v>
+      </c>
+      <c r="G5">
+        <v>1148.5513954099199</v>
+      </c>
+      <c r="H5">
+        <v>323765665792</v>
+      </c>
+      <c r="I5">
+        <v>-6.2188638796799998</v>
+      </c>
+      <c r="J5">
+        <v>-141.97623140351999</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>242.54511734784001</v>
+      </c>
+      <c r="M5">
+        <v>-35.25930442752</v>
+      </c>
+      <c r="N5">
+        <v>59.108472545280001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>2723843.5</v>
+      </c>
+      <c r="C6">
+        <v>18.009608033279999</v>
+      </c>
+      <c r="D6">
+        <v>2.3760338073599998</v>
+      </c>
+      <c r="E6">
+        <v>20.385641840640002</v>
+      </c>
+      <c r="F6">
+        <v>15.63357198336</v>
+      </c>
+      <c r="G6">
+        <v>29.290073917440001</v>
+      </c>
+      <c r="H6">
+        <v>64780673024</v>
+      </c>
+      <c r="I6">
+        <v>-3.0504422400000002</v>
+      </c>
+      <c r="J6">
+        <v>-5.1029318246399997</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>9.3735094732800004</v>
+      </c>
+      <c r="M6">
+        <v>-1.51792775424</v>
+      </c>
+      <c r="N6">
+        <v>-0.29779224048000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>636362.125</v>
+      </c>
+      <c r="C7">
+        <v>2.4798161203200002</v>
+      </c>
+      <c r="D7">
+        <v>0.69583272959999898</v>
+      </c>
+      <c r="E7">
+        <v>3.17564884992</v>
+      </c>
+      <c r="F7">
+        <v>1.7839836710400001</v>
+      </c>
+      <c r="G7">
+        <v>5.9822827699200003</v>
+      </c>
+      <c r="H7">
+        <v>13952835584</v>
+      </c>
+      <c r="I7">
+        <v>-2.6868319410000001E-2</v>
+      </c>
+      <c r="J7">
+        <v>-0.72830801184000005</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>1.4591649734400001</v>
+      </c>
+      <c r="M7">
+        <v>-0.33778784256</v>
+      </c>
+      <c r="N7">
+        <v>0.36620079744</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>22070840</v>
+      </c>
+      <c r="C8">
+        <v>683.04997277183998</v>
+      </c>
+      <c r="D8">
+        <v>193.41863480832001</v>
+      </c>
+      <c r="E8">
+        <v>876.46860758015998</v>
+      </c>
+      <c r="F8">
+        <v>489.63133151616</v>
+      </c>
+      <c r="G8">
+        <v>1440.3786306432</v>
+      </c>
+      <c r="H8">
+        <v>572193243136</v>
+      </c>
+      <c r="I8">
+        <v>-15.090409395884199</v>
+      </c>
+      <c r="J8">
+        <v>-172.85757677088</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>295.16832908736001</v>
+      </c>
+      <c r="M8">
+        <v>-44.445802687679901</v>
+      </c>
+      <c r="N8">
+        <v>62.792297685119998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1772,22 +2853,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1795,169 +2877,196 @@
         <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
       <c r="B2">
-        <f>ROUND(Baseline!B2,-1)</f>
+        <f>ROUND(EEZ.bl!C2,-1)</f>
         <v>420</v>
       </c>
       <c r="C2">
-        <f>ROUND(Baseline!L2,-1)</f>
+        <f>EEZ.bl!C2/EEZ.bl!B2*1000000000/(365*24)</f>
+        <v>23.782581416453663</v>
+      </c>
+      <c r="D2">
+        <f>ROUND(EEZ.bl!N2,-1)</f>
         <v>90</v>
       </c>
-      <c r="D2">
-        <f>ROUND(Extraction!L2,-1)</f>
-        <v>190</v>
-      </c>
       <c r="E2">
-        <f>B2+C2</f>
-        <v>510</v>
+        <f>ROUND(EEZ.ex!N2,-1)</f>
+        <v>210</v>
       </c>
       <c r="F2">
         <f>B2+D2</f>
-        <v>610</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>510</v>
+      </c>
+      <c r="G2">
+        <f>B2+E2</f>
+        <v>630</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
       <c r="B3">
-        <f>ROUND(Baseline!B3,-1)</f>
+        <f>ROUND(EEZ.bl!C3,-1)</f>
         <v>110</v>
       </c>
       <c r="C3">
-        <f>ROUND(Baseline!L3,-1)</f>
-        <v>170</v>
+        <f>EEZ.bl!C3/EEZ.bl!B3*1000000000/(365*24)</f>
+        <v>6.3463879650826662</v>
       </c>
       <c r="D3">
-        <f>ROUND(Extraction!L3,-1)</f>
-        <v>210</v>
+        <f>ROUND(EEZ.bl!N3,-1)</f>
+        <v>180</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E8" si="0">B3+C3</f>
-        <v>280</v>
+        <f>ROUND(EEZ.ex!N3,-1)</f>
+        <v>230</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F8" si="1">B3+D3</f>
-        <v>320</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <f t="shared" ref="F3:F7" si="0">B3+D3</f>
+        <v>290</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G7" si="1">B3+E3</f>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>26</v>
       </c>
       <c r="B4">
-        <f>ROUND(Baseline!B4,-1)</f>
+        <f>ROUND(EEZ.bl!C4,-1)</f>
         <v>370</v>
       </c>
       <c r="C4">
-        <f>ROUND(Baseline!L4,-1)</f>
+        <f>EEZ.bl!C4/EEZ.bl!B4*1000000000/(365*24)</f>
+        <v>9.6378774163366643</v>
+      </c>
+      <c r="D4">
+        <f>ROUND(EEZ.bl!N4,-1)</f>
         <v>10</v>
       </c>
-      <c r="D4">
-        <f>ROUND(Extraction!L4,-1)</f>
-        <v>90</v>
-      </c>
       <c r="E4">
+        <f>ROUND(EEZ.ex!N4,-1)</f>
+        <v>100</v>
+      </c>
+      <c r="F4">
         <f t="shared" si="0"/>
         <v>380</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <f t="shared" si="1"/>
-        <v>460</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>27</v>
       </c>
       <c r="B5">
-        <f>ROUND(Baseline!B5,-1)</f>
+        <f>ROUND(EEZ.bl!C5,-1)</f>
         <v>1040</v>
       </c>
       <c r="C5">
-        <f>ROUND(Baseline!L5,-1)</f>
-        <v>960</v>
+        <f>EEZ.bl!C5/EEZ.bl!B5*1000000000/(365*24)</f>
+        <v>21.388166914612349</v>
       </c>
       <c r="D5">
-        <f>ROUND(Extraction!L5,-1)</f>
-        <v>1390</v>
+        <f>ROUND(EEZ.bl!N5,-1)</f>
+        <v>990</v>
       </c>
       <c r="E5">
+        <f>ROUND(EEZ.ex!N5,-1)</f>
+        <v>1510</v>
+      </c>
+      <c r="F5">
         <f t="shared" si="0"/>
-        <v>2000</v>
-      </c>
-      <c r="F5">
+        <v>2030</v>
+      </c>
+      <c r="G5">
         <f t="shared" si="1"/>
-        <v>2430</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>2550</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>28</v>
       </c>
       <c r="B6">
-        <f>ROUND(Baseline!B6,0)</f>
+        <f>ROUND(EEZ.bl!C6,0)</f>
         <v>13</v>
       </c>
       <c r="C6">
-        <f>ROUND(Baseline!L6,0)</f>
-        <v>55</v>
+        <f>EEZ.bl!C6/EEZ.bl!B6*1000000000/(365*24)</f>
+        <v>1.6063906282170288</v>
       </c>
       <c r="D6">
-        <f>ROUND(Extraction!L6,0)</f>
-        <v>55</v>
+        <f>ROUND(EEZ.bl!N6,0)</f>
+        <v>56</v>
       </c>
       <c r="E6">
+        <f>ROUND(EEZ.ex!N6,0)</f>
+        <v>57</v>
+      </c>
+      <c r="F6">
         <f t="shared" si="0"/>
-        <v>68</v>
-      </c>
-      <c r="F6">
+        <v>69</v>
+      </c>
+      <c r="G6">
         <f t="shared" si="1"/>
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>29</v>
       </c>
       <c r="B7">
-        <f>ROUND(Baseline!B7,0)</f>
+        <f>ROUND(EEZ.bl!C7,0)</f>
         <v>6</v>
       </c>
       <c r="C7">
-        <f>ROUND(Baseline!L7,0)</f>
+        <f>EEZ.bl!C7/EEZ.bl!B7*1000000000/(365*24)</f>
+        <v>6.4623957703645418</v>
+      </c>
+      <c r="D7">
+        <f>ROUND(EEZ.bl!N7,0)</f>
         <v>11</v>
       </c>
-      <c r="D7">
-        <f>ROUND(Extraction!L7,0)</f>
-        <v>26</v>
-      </c>
       <c r="E7">
+        <f>ROUND(EEZ.ex!N7,0)</f>
+        <v>27</v>
+      </c>
+      <c r="F7">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <f t="shared" si="1"/>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -1966,20 +3075,24 @@
         <v>1959</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" ref="C8:F8" si="2">SUM(C2:C7)</f>
-        <v>1296</v>
+        <f>EEZ.bl!C8/EEZ.bl!B8*1000000000/(365*24)</f>
+        <v>14.996700460691404</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="2"/>
-        <v>1961</v>
+        <f t="shared" ref="D8:G8" si="2">SUM(D2:D7)</f>
+        <v>1337</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="2"/>
-        <v>3255</v>
+        <v>2134</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="2"/>
-        <v>3920</v>
+        <v>3296</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="2"/>
+        <v>4093</v>
       </c>
     </row>
   </sheetData>
@@ -1987,12 +3100,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2022,7 +3135,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
-        <f>Summary!A2</f>
+        <f>EEZ.Summary!A2</f>
         <v>West Coast</v>
       </c>
       <c r="B2">
@@ -2030,29 +3143,29 @@
         <v>590</v>
       </c>
       <c r="C2">
-        <f>Summary!E2</f>
+        <f>EEZ.Summary!F2</f>
         <v>510</v>
       </c>
       <c r="D2" cm="1">
-        <f t="array" ref="D2:D8">Summary!F2:F8</f>
-        <v>610</v>
+        <f t="array" ref="D2:D8">EEZ.Summary!G2:G8</f>
+        <v>630</v>
       </c>
       <c r="E2">
         <f>AVERAGE(C2:D2)</f>
-        <v>560</v>
-      </c>
-      <c r="F2" s="3">
+        <v>570</v>
+      </c>
+      <c r="F2" s="2">
         <f t="shared" ref="F2:F3" si="0">(E2-B2)/B2</f>
-        <v>-5.0847457627118647E-2</v>
-      </c>
-      <c r="G2" s="3">
+        <v>-3.3898305084745763E-2</v>
+      </c>
+      <c r="G2" s="2">
         <f>(D2-E2)/B2</f>
-        <v>8.4745762711864403E-2</v>
+        <v>0.10169491525423729</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
-        <f>Summary!A3</f>
+        <f>EEZ.Summary!A3</f>
         <v>East Coast</v>
       </c>
       <c r="B3">
@@ -2060,28 +3173,28 @@
         <v>240</v>
       </c>
       <c r="C3">
-        <f>Summary!E3</f>
-        <v>280</v>
+        <f>EEZ.Summary!F3</f>
+        <v>290</v>
       </c>
       <c r="D3">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E8" si="1">AVERAGE(C3:D3)</f>
-        <v>300</v>
-      </c>
-      <c r="F3" s="3">
+        <v>315</v>
+      </c>
+      <c r="F3" s="2">
         <f t="shared" si="0"/>
-        <v>0.25</v>
-      </c>
-      <c r="G3" s="3">
+        <v>0.3125</v>
+      </c>
+      <c r="G3" s="2">
         <f t="shared" ref="G3:G8" si="2">(D3-E3)/B3</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
-        <f>Summary!A4</f>
+        <f>EEZ.Summary!A4</f>
         <v>Hawaii</v>
       </c>
       <c r="B4">
@@ -2089,28 +3202,28 @@
         <v>130</v>
       </c>
       <c r="C4">
-        <f>Summary!E4</f>
+        <f>EEZ.Summary!F4</f>
         <v>380</v>
       </c>
       <c r="D4">
-        <v>460</v>
+        <v>470</v>
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
-        <v>420</v>
-      </c>
-      <c r="F4" s="3">
+        <v>425</v>
+      </c>
+      <c r="F4" s="2">
         <f>(E4-B4)/B4</f>
-        <v>2.2307692307692308</v>
-      </c>
-      <c r="G4" s="3">
+        <v>2.2692307692307692</v>
+      </c>
+      <c r="G4" s="2">
         <f t="shared" si="2"/>
-        <v>0.30769230769230771</v>
+        <v>0.34615384615384615</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
-        <f>Summary!A5</f>
+        <f>EEZ.Summary!A5</f>
         <v>Alaska</v>
       </c>
       <c r="B5">
@@ -2118,28 +3231,28 @@
         <v>1570</v>
       </c>
       <c r="C5">
-        <f>Summary!E5</f>
-        <v>2000</v>
+        <f>EEZ.Summary!F5</f>
+        <v>2030</v>
       </c>
       <c r="D5">
-        <v>2430</v>
+        <v>2550</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>2215</v>
-      </c>
-      <c r="F5" s="3">
+        <v>2290</v>
+      </c>
+      <c r="F5" s="2">
         <f t="shared" ref="F5:F8" si="3">(E5-B5)/B5</f>
-        <v>0.41082802547770703</v>
-      </c>
-      <c r="G5" s="3">
+        <v>0.45859872611464969</v>
+      </c>
+      <c r="G5" s="2">
         <f t="shared" si="2"/>
-        <v>0.13694267515923567</v>
+        <v>0.16560509554140126</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
-        <f>Summary!A6</f>
+        <f>EEZ.Summary!A6</f>
         <v>Gulf of Mexico</v>
       </c>
       <c r="B6">
@@ -2147,28 +3260,28 @@
         <v>80</v>
       </c>
       <c r="C6">
-        <f>Summary!E6</f>
-        <v>68</v>
+        <f>EEZ.Summary!F6</f>
+        <v>69</v>
       </c>
       <c r="D6">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>68</v>
-      </c>
-      <c r="F6" s="3">
+        <v>69.5</v>
+      </c>
+      <c r="F6" s="2">
         <f t="shared" si="3"/>
-        <v>-0.15</v>
-      </c>
-      <c r="G6" s="3">
+        <v>-0.13125000000000001</v>
+      </c>
+      <c r="G6" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.2500000000000003E-3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
-        <f>Summary!A7</f>
+        <f>EEZ.Summary!A7</f>
         <v>Puerto Rico + US V.I.</v>
       </c>
       <c r="B7">
@@ -2176,28 +3289,28 @@
         <v>30</v>
       </c>
       <c r="C7">
-        <f>Summary!E7</f>
+        <f>EEZ.Summary!F7</f>
         <v>17</v>
       </c>
       <c r="D7">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>24.5</v>
-      </c>
-      <c r="F7" s="3">
+        <v>25</v>
+      </c>
+      <c r="F7" s="2">
         <f t="shared" si="3"/>
-        <v>-0.18333333333333332</v>
-      </c>
-      <c r="G7" s="3">
+        <v>-0.16666666666666666</v>
+      </c>
+      <c r="G7" s="2">
         <f t="shared" si="2"/>
-        <v>0.25</v>
+        <v>0.26666666666666666</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
-        <f>Summary!A8</f>
+        <f>EEZ.Summary!A8</f>
         <v>TOTAL</v>
       </c>
       <c r="B8">
@@ -2205,23 +3318,23 @@
         <v>2640</v>
       </c>
       <c r="C8">
-        <f>Summary!E8</f>
-        <v>3255</v>
+        <f>EEZ.Summary!F8</f>
+        <v>3296</v>
       </c>
       <c r="D8">
-        <v>3920</v>
+        <v>4093</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>3587.5</v>
-      </c>
-      <c r="F8" s="3">
+        <v>3694.5</v>
+      </c>
+      <c r="F8" s="2">
         <f t="shared" si="3"/>
-        <v>0.35890151515151514</v>
-      </c>
-      <c r="G8" s="3">
+        <v>0.39943181818181817</v>
+      </c>
+      <c r="G8" s="2">
         <f t="shared" si="2"/>
-        <v>0.1259469696969697</v>
+        <v>0.15094696969696969</v>
       </c>
     </row>
   </sheetData>
@@ -2229,11 +3342,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -2244,7 +3357,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="str" cm="1">
-        <f t="array" ref="A1:A8">Summary!A1:A8</f>
+        <f t="array" ref="A1:A8">EEZ.Summary!A1:A8</f>
         <v>Region</v>
       </c>
       <c r="B1" t="s">
@@ -2262,18 +3375,18 @@
         <v>West Coast</v>
       </c>
       <c r="B2">
-        <f>ROUND(Baseline!C2,-1)</f>
+        <f>ROUND(EEZ.bl!D2,-1)</f>
         <v>60</v>
       </c>
       <c r="C2">
-        <f>Summary!B2</f>
+        <f>EEZ.Summary!B2</f>
         <v>420</v>
       </c>
       <c r="D2">
-        <f>Summary!C2</f>
+        <f>EEZ.Summary!D2</f>
         <v>90</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <f>(B2-D2/2)/C2</f>
         <v>3.5714285714285712E-2</v>
       </c>
@@ -2283,20 +3396,20 @@
         <v>East Coast</v>
       </c>
       <c r="B3">
-        <f>ROUND(Baseline!C3,-1)</f>
+        <f>ROUND(EEZ.bl!D3,-1)</f>
         <v>110</v>
       </c>
       <c r="C3">
-        <f>Summary!B3</f>
+        <f>EEZ.Summary!B3</f>
         <v>110</v>
       </c>
       <c r="D3">
-        <f>Summary!C3</f>
-        <v>170</v>
-      </c>
-      <c r="E3" s="3">
+        <f>EEZ.Summary!D3</f>
+        <v>180</v>
+      </c>
+      <c r="E3" s="2">
         <f t="shared" ref="E3:E7" si="0">(B3-D3/2)/C3</f>
-        <v>0.22727272727272727</v>
+        <v>0.18181818181818182</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2304,18 +3417,18 @@
         <v>Hawaii</v>
       </c>
       <c r="B4">
-        <f>ROUND(Baseline!C4,-1)</f>
+        <f>ROUND(EEZ.bl!D4,-1)</f>
         <v>290</v>
       </c>
       <c r="C4">
-        <f>Summary!B4</f>
+        <f>EEZ.Summary!B4</f>
         <v>370</v>
       </c>
       <c r="D4">
-        <f>Summary!C4</f>
+        <f>EEZ.Summary!D4</f>
         <v>10</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <f t="shared" si="0"/>
         <v>0.77027027027027029</v>
       </c>
@@ -2325,20 +3438,20 @@
         <v>Alaska</v>
       </c>
       <c r="B5">
-        <f>ROUND(Baseline!C5,-1)</f>
+        <f>ROUND(EEZ.bl!D5,-1)</f>
         <v>610</v>
       </c>
       <c r="C5">
-        <f>Summary!B5</f>
+        <f>EEZ.Summary!B5</f>
         <v>1040</v>
       </c>
       <c r="D5">
-        <f>Summary!C5</f>
-        <v>960</v>
-      </c>
-      <c r="E5" s="3">
+        <f>EEZ.Summary!D5</f>
+        <v>990</v>
+      </c>
+      <c r="E5" s="2">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>0.11057692307692307</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2346,20 +3459,20 @@
         <v>Gulf of Mexico</v>
       </c>
       <c r="B6">
-        <f>ROUND(Baseline!C6,0)</f>
+        <f>ROUND(EEZ.bl!D6,0)</f>
         <v>15</v>
       </c>
       <c r="C6">
-        <f>Summary!B6</f>
+        <f>EEZ.Summary!B6</f>
         <v>13</v>
       </c>
       <c r="D6">
-        <f>Summary!C6</f>
-        <v>55</v>
-      </c>
-      <c r="E6" s="3">
+        <f>EEZ.Summary!D6</f>
+        <v>56</v>
+      </c>
+      <c r="E6" s="2">
         <f t="shared" si="0"/>
-        <v>-0.96153846153846156</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -2367,18 +3480,18 @@
         <v>Puerto Rico + US V.I.</v>
       </c>
       <c r="B7">
-        <f>ROUND(Baseline!C7,0)</f>
+        <f>ROUND(EEZ.bl!D7,0)</f>
         <v>2</v>
       </c>
       <c r="C7">
-        <f>Summary!B7</f>
+        <f>EEZ.Summary!B7</f>
         <v>6</v>
       </c>
       <c r="D7">
-        <f>Summary!C7</f>
+        <f>EEZ.Summary!D7</f>
         <v>11</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <f t="shared" si="0"/>
         <v>-0.58333333333333337</v>
       </c>
@@ -2388,16 +3501,263 @@
         <v>TOTAL</v>
       </c>
       <c r="B8">
-        <f>ROUND(Baseline!C8,-1)</f>
+        <f>ROUND(EEZ.bl!D8,-1)</f>
         <v>1080</v>
       </c>
       <c r="C8">
-        <f>Summary!B8</f>
+        <f>EEZ.Summary!B8</f>
         <v>1959</v>
       </c>
       <c r="D8">
-        <f>Summary!C8</f>
-        <v>1296</v>
+        <f>EEZ.Summary!D8</f>
+        <v>1337</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F893EFA9-E3BF-F249-9404-9C034DB18919}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <f>ROUND(Near.bl!C2,-1)</f>
+        <v>410</v>
+      </c>
+      <c r="C2">
+        <f>Near.bl!C2/Near.bl!B2*1000000000/(365*24)</f>
+        <v>18.526980777148271</v>
+      </c>
+      <c r="D2">
+        <f>ROUND(Near.bl!N2,-1)</f>
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>ROUND(Near.ex!N2,-1)</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>B2+D2</f>
+        <v>410</v>
+      </c>
+      <c r="G2">
+        <f>B2+E2</f>
+        <v>410</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3">
+        <f>ROUND(Near.bl!C3,-1)</f>
+        <v>90</v>
+      </c>
+      <c r="C3">
+        <f>Near.bl!C3/Near.bl!B3*1000000000/(365*24)</f>
+        <v>3.323639053273399</v>
+      </c>
+      <c r="D3">
+        <f>ROUND(Near.bl!N3,-1)</f>
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f>ROUND(Near.ex!N3,-1)</f>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F7" si="0">B3+D3</f>
+        <v>90</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G7" si="1">B3+E3</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4">
+        <f>ROUND(Near.bl!C4,-1)</f>
+        <v>40</v>
+      </c>
+      <c r="C4">
+        <f>Near.bl!C4/Near.bl!B4*1000000000/(365*24)</f>
+        <v>2.4715731789716493</v>
+      </c>
+      <c r="D4">
+        <f>ROUND(Near.bl!N4,-1)</f>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f>ROUND(Near.ex!N4,-1)</f>
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <f>ROUND(Near.bl!C5,-1)</f>
+        <v>1140</v>
+      </c>
+      <c r="C5">
+        <f>Near.bl!C5/Near.bl!B5*1000000000/(365*24)</f>
+        <v>11.5652459213601</v>
+      </c>
+      <c r="D5">
+        <f>ROUND(Near.bl!N5,-1)</f>
+        <v>50</v>
+      </c>
+      <c r="E5">
+        <f>ROUND(Near.ex!N5,-1)</f>
+        <v>60</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>1190</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6">
+        <f>ROUND(Near.bl!C6,-1)</f>
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <f>Near.bl!C6/Near.bl!B6*1000000000/(365*24)</f>
+        <v>1.0255056371630749</v>
+      </c>
+      <c r="D6">
+        <f>ROUND(Near.bl!N6,-1)</f>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f>ROUND(Near.ex!N6,-1)</f>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7">
+        <f>ROUND(Near.bl!C7,-1)</f>
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <f>Near.bl!C7/Near.bl!B7*1000000000/(365*24)</f>
+        <v>3.1644058514638971</v>
+      </c>
+      <c r="D7">
+        <f>ROUND(Near.bl!N7,-1)</f>
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f>ROUND(Near.ex!N7,-1)</f>
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1">
+        <f>SUM(B2:B7)</f>
+        <v>1720</v>
+      </c>
+      <c r="C8">
+        <f>Near.bl!C8/Near.bl!B8*1000000000/(365*24)</f>
+        <v>8.9131995875100376</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" ref="D8:G8" si="2">SUM(D2:D7)</f>
+        <v>50</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="2"/>
+        <v>1770</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="2"/>
+        <v>1780</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix another Hawaii bug.
</commit_message>
<xml_diff>
--- a/results/Total_Results.xlsx
+++ b/results/Total_Results.xlsx
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lkilcher/Dropbox/work/mhk/wave_res/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57EDE7B-35E9-5D41-B918-D36992C96934}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48EE774-D5DA-864D-9BC2-2B85DF91AFC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29680" yWindow="-3140" windowWidth="24640" windowHeight="14000" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27840" yWindow="-460" windowWidth="24640" windowHeight="14000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EEZ.bl" sheetId="2" r:id="rId1"/>
     <sheet name="EEZ.ex" sheetId="1" r:id="rId2"/>
     <sheet name="Near.bl" sheetId="7" r:id="rId3"/>
     <sheet name="Near.ex" sheetId="8" r:id="rId4"/>
-    <sheet name="EPRI2011" sheetId="4" r:id="rId5"/>
+    <sheet name="EPRI" sheetId="4" r:id="rId5"/>
     <sheet name="EEZ.Summary" sheetId="3" r:id="rId6"/>
     <sheet name="EEZ.COMPARE" sheetId="5" r:id="rId7"/>
-    <sheet name="one-way" sheetId="6" r:id="rId8"/>
-    <sheet name="Near.Summary" sheetId="9" r:id="rId9"/>
-    <sheet name="Near.COMPARE" sheetId="10" r:id="rId10"/>
+    <sheet name="Near.Summary" sheetId="9" r:id="rId8"/>
+    <sheet name="Near.COMPARE" sheetId="10" r:id="rId9"/>
+    <sheet name="one-way" sheetId="6" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="45">
   <si>
     <t>bdir</t>
   </si>
@@ -174,9 +174,6 @@
     <t>Upper</t>
   </si>
   <si>
-    <t>EPRI</t>
-  </si>
-  <si>
     <t>Onshore</t>
   </si>
   <si>
@@ -190,6 +187,15 @@
   </si>
   <si>
     <t>Flux (kW/m)</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>EPRI 2011</t>
+  </si>
+  <si>
+    <t>EPRI 2004</t>
   </si>
 </sst>
 </file>
@@ -1045,7 +1051,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1063,7 +1069,7 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -1426,246 +1432,174 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FFF2529-D61C-C04A-AE20-738CA7021AB0}">
-  <dimension ref="A1:G8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="9.5" customWidth="1"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="str" cm="1">
+        <f t="array" ref="A1:A8">EEZ.Summary!A1:A8</f>
+        <v>Region</v>
+      </c>
       <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
-        <v>35</v>
-      </c>
       <c r="D1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
-        <f>EEZ.Summary!A2</f>
         <v>West Coast</v>
       </c>
       <c r="B2">
-        <f>EPRI2011!B2</f>
-        <v>590</v>
+        <f>ROUND(EEZ.bl!D2,-1)</f>
+        <v>60</v>
       </c>
       <c r="C2">
-        <f>Near.Summary!F2</f>
-        <v>410</v>
+        <f>EEZ.Summary!B2</f>
+        <v>420</v>
       </c>
       <c r="D2">
-        <f>Near.Summary!G2</f>
-        <v>410</v>
-      </c>
-      <c r="E2">
-        <f>AVERAGE(C2:D2)</f>
-        <v>410</v>
-      </c>
-      <c r="F2" s="2">
-        <f t="shared" ref="F2:F3" si="0">(E2-B2)/B2</f>
-        <v>-0.30508474576271188</v>
-      </c>
-      <c r="G2" s="2">
-        <f>(D2-E2)/B2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <f>EEZ.Summary!D2</f>
+        <v>90</v>
+      </c>
+      <c r="E2" s="2">
+        <f>(B2-D2/2)/C2</f>
+        <v>3.5714285714285712E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
-        <f>EEZ.Summary!A3</f>
         <v>East Coast</v>
       </c>
       <c r="B3">
-        <f>EPRI2011!B3</f>
-        <v>240</v>
+        <f>ROUND(EEZ.bl!D3,-1)</f>
+        <v>110</v>
       </c>
       <c r="C3">
-        <f>Near.Summary!F3</f>
-        <v>90</v>
+        <f>EEZ.Summary!B3</f>
+        <v>110</v>
       </c>
       <c r="D3">
-        <f>Near.Summary!G3</f>
-        <v>90</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E8" si="1">AVERAGE(C3:D3)</f>
-        <v>90</v>
-      </c>
-      <c r="F3" s="2">
+        <f>EEZ.Summary!D3</f>
+        <v>180</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E7" si="0">(B3-D3/2)/C3</f>
+        <v>0.18181818181818182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <v>Hawaii</v>
+      </c>
+      <c r="B4">
+        <f>ROUND(EEZ.bl!D4,-1)</f>
+        <v>290</v>
+      </c>
+      <c r="C4">
+        <f>EEZ.Summary!B4</f>
+        <v>370</v>
+      </c>
+      <c r="D4">
+        <f>EEZ.Summary!D4</f>
+        <v>10</v>
+      </c>
+      <c r="E4" s="2">
         <f t="shared" si="0"/>
-        <v>-0.625</v>
-      </c>
-      <c r="G3" s="2">
-        <f t="shared" ref="G3:G8" si="2">(D3-E3)/B3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="str">
-        <f>EEZ.Summary!A4</f>
-        <v>Hawaii</v>
-      </c>
-      <c r="B4">
-        <f>EPRI2011!B4</f>
-        <v>130</v>
-      </c>
-      <c r="C4">
-        <f>Near.Summary!F4</f>
-        <v>40</v>
-      </c>
-      <c r="D4">
-        <f>Near.Summary!G4</f>
-        <v>40</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="F4" s="2">
-        <f>(E4-B4)/B4</f>
-        <v>-0.69230769230769229</v>
-      </c>
-      <c r="G4" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.77027027027027029</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
-        <f>EEZ.Summary!A5</f>
         <v>Alaska</v>
       </c>
       <c r="B5">
-        <f>EPRI2011!B5</f>
-        <v>1570</v>
+        <f>ROUND(EEZ.bl!D5,-1)</f>
+        <v>610</v>
       </c>
       <c r="C5">
-        <f>Near.Summary!F5</f>
-        <v>1190</v>
+        <f>EEZ.Summary!B5</f>
+        <v>1040</v>
       </c>
       <c r="D5">
-        <f>Near.Summary!G5</f>
-        <v>1200</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="1"/>
-        <v>1195</v>
-      </c>
-      <c r="F5" s="2">
-        <f t="shared" ref="F5:F8" si="3">(E5-B5)/B5</f>
-        <v>-0.23885350318471338</v>
-      </c>
-      <c r="G5" s="2">
-        <f t="shared" si="2"/>
-        <v>3.1847133757961785E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <f>EEZ.Summary!D5</f>
+        <v>990</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>0.11057692307692307</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
-        <f>EEZ.Summary!A6</f>
         <v>Gulf of Mexico</v>
       </c>
       <c r="B6">
-        <f>EPRI2011!B6</f>
-        <v>80</v>
+        <f>ROUND(EEZ.bl!D6,0)</f>
+        <v>15</v>
       </c>
       <c r="C6">
-        <f>Near.Summary!F6</f>
-        <v>20</v>
+        <f>EEZ.Summary!B6</f>
+        <v>13</v>
       </c>
       <c r="D6">
-        <f>Near.Summary!G6</f>
-        <v>20</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="F6" s="2">
-        <f t="shared" si="3"/>
-        <v>-0.75</v>
-      </c>
-      <c r="G6" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <f>EEZ.Summary!D6</f>
+        <v>56</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
-        <f>EEZ.Summary!A7</f>
         <v>Puerto Rico + US V.I.</v>
       </c>
       <c r="B7">
-        <f>EPRI2011!B7</f>
-        <v>30</v>
+        <f>ROUND(EEZ.bl!D7,0)</f>
+        <v>2</v>
       </c>
       <c r="C7">
-        <f>Near.Summary!F7</f>
-        <v>20</v>
+        <f>EEZ.Summary!B7</f>
+        <v>6</v>
       </c>
       <c r="D7">
-        <f>Near.Summary!G7</f>
-        <v>20</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="F7" s="2">
-        <f t="shared" si="3"/>
-        <v>-0.33333333333333331</v>
-      </c>
-      <c r="G7" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <f>EEZ.Summary!D7</f>
+        <v>11</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
-        <f>EEZ.Summary!A8</f>
         <v>TOTAL</v>
       </c>
       <c r="B8">
-        <f>EPRI2011!B8</f>
-        <v>2640</v>
+        <f>ROUND(EEZ.bl!D8,-1)</f>
+        <v>1080</v>
       </c>
       <c r="C8">
-        <f>Near.Summary!F8</f>
-        <v>1770</v>
+        <f>EEZ.Summary!B8</f>
+        <v>1959</v>
       </c>
       <c r="D8">
-        <f>Near.Summary!G8</f>
-        <v>1780</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="1"/>
-        <v>1775</v>
-      </c>
-      <c r="F8" s="2">
-        <f t="shared" si="3"/>
-        <v>-0.32765151515151514</v>
-      </c>
-      <c r="G8" s="2">
-        <f t="shared" si="2"/>
-        <v>1.893939393939394E-3</v>
+        <f>EEZ.Summary!D8</f>
+        <v>1337</v>
       </c>
     </row>
   </sheetData>
@@ -1696,7 +1630,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1714,7 +1648,7 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -2052,15 +1986,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51B6B5B9-50BB-3A4E-98D2-F24B327EABE8}">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2078,7 +2012,7 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -2195,16 +2129,16 @@
         <v>1749916.125</v>
       </c>
       <c r="C4">
-        <v>37.887400857599999</v>
+        <v>117.97534961664</v>
       </c>
       <c r="D4">
-        <v>117.97534513152</v>
+        <v>37.887396372479998</v>
       </c>
       <c r="E4">
         <v>155.86274598911999</v>
       </c>
       <c r="F4">
-        <v>-80.087953244160005</v>
+        <v>80.087953244160005</v>
       </c>
       <c r="G4">
         <v>261.07921195007998</v>
@@ -2371,16 +2305,16 @@
         <v>22070840</v>
       </c>
       <c r="C8">
-        <v>1723.2829853798401</v>
+        <v>1803.3709341388801</v>
       </c>
       <c r="D8">
-        <v>382.82695339007898</v>
+        <v>302.73900463103899</v>
       </c>
       <c r="E8">
         <v>2106.1099387699201</v>
       </c>
       <c r="F8">
-        <v>1340.4563650099201</v>
+        <v>1500.63227149824</v>
       </c>
       <c r="G8">
         <v>3231.2181860351998</v>
@@ -2417,14 +2351,14 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2442,7 +2376,7 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -2559,16 +2493,16 @@
         <v>1749916.125</v>
       </c>
       <c r="C4">
-        <v>7.5513812582400002</v>
+        <v>17.447882634239999</v>
       </c>
       <c r="D4">
-        <v>17.447881512959999</v>
+        <v>7.5513801369599998</v>
       </c>
       <c r="E4">
         <v>24.999262771200002</v>
       </c>
       <c r="F4">
-        <v>-9.8965002547199994</v>
+        <v>9.8965002547199994</v>
       </c>
       <c r="G4">
         <v>43.753372692479999</v>
@@ -2735,16 +2669,16 @@
         <v>22070840</v>
       </c>
       <c r="C8">
-        <v>683.04997277183998</v>
+        <v>692.94647414784004</v>
       </c>
       <c r="D8">
-        <v>193.41863480832001</v>
+        <v>183.52213343232</v>
       </c>
       <c r="E8">
         <v>876.46860758015998</v>
       </c>
       <c r="F8">
-        <v>489.63133151616</v>
+        <v>509.42433202559999</v>
       </c>
       <c r="G8">
         <v>1440.3786306432</v>
@@ -2778,73 +2712,94 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D2" sqref="D2:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1">
+        <v>2004</v>
+      </c>
+      <c r="C1">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
       <c r="B2">
+        <v>440</v>
+      </c>
+      <c r="C2">
         <v>590</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3">
+        <v>110</v>
+      </c>
+      <c r="C3">
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4">
+        <v>300</v>
+      </c>
+      <c r="C4">
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5">
+        <v>1250</v>
+      </c>
+      <c r="C5">
         <v>1570</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8">
-        <f>SUM(B2:B7)</f>
+      <c r="C8">
+        <f>SUM(C2:C7)</f>
         <v>2640</v>
       </c>
     </row>
@@ -2877,7 +2832,7 @@
         <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>22</v>
@@ -3102,237 +3057,299 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="9.5" customWidth="1"/>
+    <col min="7" max="7" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>33</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>EEZ.Summary!A2</f>
         <v>West Coast</v>
       </c>
       <c r="B2">
-        <f>EPRI2011!B2</f>
+        <f>EPRI!B2</f>
+        <v>440</v>
+      </c>
+      <c r="C2">
+        <f>EPRI!C2</f>
         <v>590</v>
       </c>
-      <c r="C2">
+      <c r="D2">
+        <f>EEZ.Summary!B2</f>
+        <v>420</v>
+      </c>
+      <c r="E2">
         <f>EEZ.Summary!F2</f>
         <v>510</v>
       </c>
-      <c r="D2" cm="1">
-        <f t="array" ref="D2:D8">EEZ.Summary!G2:G8</f>
+      <c r="F2" cm="1">
+        <f t="array" ref="F2:F8">EEZ.Summary!G2:G8</f>
         <v>630</v>
       </c>
-      <c r="E2">
-        <f>AVERAGE(C2:D2)</f>
+      <c r="G2">
+        <f>AVERAGE(E2:F2)</f>
         <v>570</v>
       </c>
-      <c r="F2" s="2">
-        <f t="shared" ref="F2:F3" si="0">(E2-B2)/B2</f>
+      <c r="H2" s="2">
+        <f t="shared" ref="H2:H3" si="0">(G2-C2)/C2</f>
         <v>-3.3898305084745763E-2</v>
       </c>
-      <c r="G2" s="2">
-        <f>(D2-E2)/B2</f>
+      <c r="I2" s="2">
+        <f>(F2-G2)/C2</f>
         <v>0.10169491525423729</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>EEZ.Summary!A3</f>
         <v>East Coast</v>
       </c>
       <c r="B3">
-        <f>EPRI2011!B3</f>
+        <f>EPRI!B3</f>
+        <v>110</v>
+      </c>
+      <c r="C3">
+        <f>EPRI!C3</f>
         <v>240</v>
       </c>
-      <c r="C3">
+      <c r="D3">
+        <f>EEZ.Summary!B3</f>
+        <v>110</v>
+      </c>
+      <c r="E3">
         <f>EEZ.Summary!F3</f>
         <v>290</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>340</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E8" si="1">AVERAGE(C3:D3)</f>
+      <c r="G3">
+        <f t="shared" ref="G3:G8" si="1">AVERAGE(E3:F3)</f>
         <v>315</v>
       </c>
-      <c r="F3" s="2">
+      <c r="H3" s="2">
         <f t="shared" si="0"/>
         <v>0.3125</v>
       </c>
-      <c r="G3" s="2">
-        <f t="shared" ref="G3:G8" si="2">(D3-E3)/B3</f>
+      <c r="I3" s="2">
+        <f t="shared" ref="I3:I8" si="2">(F3-G3)/C3</f>
         <v>0.10416666666666667</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>EEZ.Summary!A4</f>
         <v>Hawaii</v>
       </c>
       <c r="B4">
-        <f>EPRI2011!B4</f>
+        <f>EPRI!B4</f>
+        <v>300</v>
+      </c>
+      <c r="C4">
+        <f>EPRI!C4</f>
         <v>130</v>
       </c>
-      <c r="C4">
+      <c r="D4">
+        <f>EEZ.Summary!B4</f>
+        <v>370</v>
+      </c>
+      <c r="E4">
         <f>EEZ.Summary!F4</f>
         <v>380</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>470</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <f t="shared" si="1"/>
         <v>425</v>
       </c>
-      <c r="F4" s="2">
-        <f>(E4-B4)/B4</f>
+      <c r="H4" s="2">
+        <f>(G4-C4)/C4</f>
         <v>2.2692307692307692</v>
       </c>
-      <c r="G4" s="2">
+      <c r="I4" s="2">
         <f t="shared" si="2"/>
         <v>0.34615384615384615</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f>EEZ.Summary!A5</f>
         <v>Alaska</v>
       </c>
       <c r="B5">
-        <f>EPRI2011!B5</f>
+        <f>EPRI!B5</f>
+        <v>1250</v>
+      </c>
+      <c r="C5">
+        <f>EPRI!C5</f>
         <v>1570</v>
       </c>
-      <c r="C5">
+      <c r="D5">
+        <f>EEZ.Summary!B5</f>
+        <v>1040</v>
+      </c>
+      <c r="E5">
         <f>EEZ.Summary!F5</f>
         <v>2030</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>2550</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <f t="shared" si="1"/>
         <v>2290</v>
       </c>
-      <c r="F5" s="2">
-        <f t="shared" ref="F5:F8" si="3">(E5-B5)/B5</f>
+      <c r="H5" s="2">
+        <f t="shared" ref="H5:H8" si="3">(G5-C5)/C5</f>
         <v>0.45859872611464969</v>
       </c>
-      <c r="G5" s="2">
+      <c r="I5" s="2">
         <f t="shared" si="2"/>
         <v>0.16560509554140126</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f>EEZ.Summary!A6</f>
         <v>Gulf of Mexico</v>
       </c>
-      <c r="B6">
-        <f>EPRI2011!B6</f>
+      <c r="B6" t="str">
+        <f>EPRI!B6</f>
+        <v>N/A</v>
+      </c>
+      <c r="C6">
+        <f>EPRI!C6</f>
         <v>80</v>
       </c>
-      <c r="C6">
+      <c r="D6">
+        <f>EEZ.Summary!B6</f>
+        <v>13</v>
+      </c>
+      <c r="E6">
         <f>EEZ.Summary!F6</f>
         <v>69</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <v>70</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <f t="shared" si="1"/>
         <v>69.5</v>
       </c>
-      <c r="F6" s="2">
+      <c r="H6" s="2">
         <f t="shared" si="3"/>
         <v>-0.13125000000000001</v>
       </c>
-      <c r="G6" s="2">
+      <c r="I6" s="2">
         <f t="shared" si="2"/>
         <v>6.2500000000000003E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f>EEZ.Summary!A7</f>
         <v>Puerto Rico + US V.I.</v>
       </c>
-      <c r="B7">
-        <f>EPRI2011!B7</f>
+      <c r="B7" t="str">
+        <f>EPRI!B7</f>
+        <v>N/A</v>
+      </c>
+      <c r="C7">
+        <f>EPRI!C7</f>
         <v>30</v>
       </c>
-      <c r="C7">
+      <c r="D7">
+        <f>EEZ.Summary!B7</f>
+        <v>6</v>
+      </c>
+      <c r="E7">
         <f>EEZ.Summary!F7</f>
         <v>17</v>
       </c>
-      <c r="D7">
+      <c r="F7">
         <v>33</v>
       </c>
-      <c r="E7">
+      <c r="G7">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="F7" s="2">
+      <c r="H7" s="2">
         <f t="shared" si="3"/>
         <v>-0.16666666666666666</v>
       </c>
-      <c r="G7" s="2">
+      <c r="I7" s="2">
         <f t="shared" si="2"/>
         <v>0.26666666666666666</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f>EEZ.Summary!A8</f>
         <v>TOTAL</v>
       </c>
       <c r="B8">
-        <f>EPRI2011!B8</f>
+        <f>SUM(B2:B5)</f>
+        <v>2100</v>
+      </c>
+      <c r="C8">
+        <f>EPRI!C8</f>
         <v>2640</v>
       </c>
-      <c r="C8">
+      <c r="D8">
+        <f>EEZ.Summary!B8</f>
+        <v>1959</v>
+      </c>
+      <c r="E8">
         <f>EEZ.Summary!F8</f>
         <v>3296</v>
       </c>
-      <c r="D8">
+      <c r="F8">
         <v>4093</v>
       </c>
-      <c r="E8">
+      <c r="G8">
         <f t="shared" si="1"/>
         <v>3694.5</v>
       </c>
-      <c r="F8" s="2">
+      <c r="H8" s="2">
         <f t="shared" si="3"/>
         <v>0.39943181818181817</v>
       </c>
-      <c r="G8" s="2">
+      <c r="I8" s="2">
         <f t="shared" si="2"/>
         <v>0.15094696969696969</v>
       </c>
@@ -3343,187 +3360,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="str" cm="1">
-        <f t="array" ref="A1:A8">EEZ.Summary!A1:A8</f>
-        <v>Region</v>
-      </c>
-      <c r="B1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="str">
-        <v>West Coast</v>
-      </c>
-      <c r="B2">
-        <f>ROUND(EEZ.bl!D2,-1)</f>
-        <v>60</v>
-      </c>
-      <c r="C2">
-        <f>EEZ.Summary!B2</f>
-        <v>420</v>
-      </c>
-      <c r="D2">
-        <f>EEZ.Summary!D2</f>
-        <v>90</v>
-      </c>
-      <c r="E2" s="2">
-        <f>(B2-D2/2)/C2</f>
-        <v>3.5714285714285712E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="str">
-        <v>East Coast</v>
-      </c>
-      <c r="B3">
-        <f>ROUND(EEZ.bl!D3,-1)</f>
-        <v>110</v>
-      </c>
-      <c r="C3">
-        <f>EEZ.Summary!B3</f>
-        <v>110</v>
-      </c>
-      <c r="D3">
-        <f>EEZ.Summary!D3</f>
-        <v>180</v>
-      </c>
-      <c r="E3" s="2">
-        <f t="shared" ref="E3:E7" si="0">(B3-D3/2)/C3</f>
-        <v>0.18181818181818182</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="str">
-        <v>Hawaii</v>
-      </c>
-      <c r="B4">
-        <f>ROUND(EEZ.bl!D4,-1)</f>
-        <v>290</v>
-      </c>
-      <c r="C4">
-        <f>EEZ.Summary!B4</f>
-        <v>370</v>
-      </c>
-      <c r="D4">
-        <f>EEZ.Summary!D4</f>
-        <v>10</v>
-      </c>
-      <c r="E4" s="2">
-        <f t="shared" si="0"/>
-        <v>0.77027027027027029</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="str">
-        <v>Alaska</v>
-      </c>
-      <c r="B5">
-        <f>ROUND(EEZ.bl!D5,-1)</f>
-        <v>610</v>
-      </c>
-      <c r="C5">
-        <f>EEZ.Summary!B5</f>
-        <v>1040</v>
-      </c>
-      <c r="D5">
-        <f>EEZ.Summary!D5</f>
-        <v>990</v>
-      </c>
-      <c r="E5" s="2">
-        <f t="shared" si="0"/>
-        <v>0.11057692307692307</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="str">
-        <v>Gulf of Mexico</v>
-      </c>
-      <c r="B6">
-        <f>ROUND(EEZ.bl!D6,0)</f>
-        <v>15</v>
-      </c>
-      <c r="C6">
-        <f>EEZ.Summary!B6</f>
-        <v>13</v>
-      </c>
-      <c r="D6">
-        <f>EEZ.Summary!D6</f>
-        <v>56</v>
-      </c>
-      <c r="E6" s="2">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="str">
-        <v>Puerto Rico + US V.I.</v>
-      </c>
-      <c r="B7">
-        <f>ROUND(EEZ.bl!D7,0)</f>
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <f>EEZ.Summary!B7</f>
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <f>EEZ.Summary!D7</f>
-        <v>11</v>
-      </c>
-      <c r="E7" s="2">
-        <f t="shared" si="0"/>
-        <v>-0.58333333333333337</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="str">
-        <v>TOTAL</v>
-      </c>
-      <c r="B8">
-        <f>ROUND(EEZ.bl!D8,-1)</f>
-        <v>1080</v>
-      </c>
-      <c r="C8">
-        <f>EEZ.Summary!B8</f>
-        <v>1959</v>
-      </c>
-      <c r="D8">
-        <f>EEZ.Summary!D8</f>
-        <v>1337</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F893EFA9-E3BF-F249-9404-9C034DB18919}">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3542,7 +3383,7 @@
         <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>22</v>
@@ -3621,11 +3462,11 @@
       </c>
       <c r="B4">
         <f>ROUND(Near.bl!C4,-1)</f>
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="C4">
         <f>Near.bl!C4/Near.bl!B4*1000000000/(365*24)</f>
-        <v>2.4715731789716493</v>
+        <v>7.6960863847117249</v>
       </c>
       <c r="D4">
         <f>ROUND(Near.bl!N4,-1)</f>
@@ -3637,11 +3478,11 @@
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="G4">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -3737,11 +3578,11 @@
       </c>
       <c r="B8" s="1">
         <f>SUM(B2:B7)</f>
-        <v>1720</v>
+        <v>1800</v>
       </c>
       <c r="C8">
         <f>Near.bl!C8/Near.bl!B8*1000000000/(365*24)</f>
-        <v>8.9131995875100376</v>
+        <v>9.3274321180344764</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" ref="D8:G8" si="2">SUM(D2:D7)</f>
@@ -3753,11 +3594,290 @@
       </c>
       <c r="F8" s="1">
         <f t="shared" si="2"/>
-        <v>1770</v>
+        <v>1850</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="2"/>
-        <v>1780</v>
+        <v>1860</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FFF2529-D61C-C04A-AE20-738CA7021AB0}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="9.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>EEZ.Summary!A2</f>
+        <v>West Coast</v>
+      </c>
+      <c r="B2">
+        <f>EPRI!B2</f>
+        <v>440</v>
+      </c>
+      <c r="C2">
+        <f>EPRI!C2</f>
+        <v>590</v>
+      </c>
+      <c r="D2">
+        <f>Near.Summary!F2</f>
+        <v>410</v>
+      </c>
+      <c r="E2">
+        <f>Near.Summary!G2</f>
+        <v>410</v>
+      </c>
+      <c r="F2">
+        <f>AVERAGE(D2:E2)</f>
+        <v>410</v>
+      </c>
+      <c r="G2" s="2">
+        <f>(F2-C2)/C2</f>
+        <v>-0.30508474576271188</v>
+      </c>
+      <c r="H2" s="2">
+        <f>(E2-F2)/C2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>EEZ.Summary!A3</f>
+        <v>East Coast</v>
+      </c>
+      <c r="B3">
+        <f>EPRI!B3</f>
+        <v>110</v>
+      </c>
+      <c r="C3">
+        <f>EPRI!C3</f>
+        <v>240</v>
+      </c>
+      <c r="D3">
+        <f>Near.Summary!F3</f>
+        <v>90</v>
+      </c>
+      <c r="E3">
+        <f>Near.Summary!G3</f>
+        <v>90</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F8" si="0">AVERAGE(D3:E3)</f>
+        <v>90</v>
+      </c>
+      <c r="G3" s="2">
+        <f>(F3-C3)/C3</f>
+        <v>-0.625</v>
+      </c>
+      <c r="H3" s="2">
+        <f>(E3-F3)/C3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f>EEZ.Summary!A4</f>
+        <v>Hawaii</v>
+      </c>
+      <c r="B4">
+        <f>EPRI!B4</f>
+        <v>300</v>
+      </c>
+      <c r="C4">
+        <f>EPRI!C4</f>
+        <v>130</v>
+      </c>
+      <c r="D4">
+        <f>Near.Summary!F4</f>
+        <v>120</v>
+      </c>
+      <c r="E4">
+        <f>Near.Summary!G4</f>
+        <v>120</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="G4" s="2">
+        <f>(F4-C4)/C4</f>
+        <v>-7.6923076923076927E-2</v>
+      </c>
+      <c r="H4" s="2">
+        <f>(E4-F4)/C4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="str">
+        <f>EEZ.Summary!A5</f>
+        <v>Alaska</v>
+      </c>
+      <c r="B5">
+        <f>EPRI!B5</f>
+        <v>1250</v>
+      </c>
+      <c r="C5">
+        <f>EPRI!C5</f>
+        <v>1570</v>
+      </c>
+      <c r="D5">
+        <f>Near.Summary!F5</f>
+        <v>1190</v>
+      </c>
+      <c r="E5">
+        <f>Near.Summary!G5</f>
+        <v>1200</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>1195</v>
+      </c>
+      <c r="G5" s="2">
+        <f>(F5-C5)/C5</f>
+        <v>-0.23885350318471338</v>
+      </c>
+      <c r="H5" s="2">
+        <f>(E5-F5)/C5</f>
+        <v>3.1847133757961785E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="str">
+        <f>EEZ.Summary!A6</f>
+        <v>Gulf of Mexico</v>
+      </c>
+      <c r="B6" t="str">
+        <f>EPRI!B6</f>
+        <v>N/A</v>
+      </c>
+      <c r="C6">
+        <f>EPRI!C6</f>
+        <v>80</v>
+      </c>
+      <c r="D6">
+        <f>Near.Summary!F6</f>
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <f>Near.Summary!G6</f>
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="G6" s="2">
+        <f>(F6-C6)/C6</f>
+        <v>-0.75</v>
+      </c>
+      <c r="H6" s="2">
+        <f>(E6-F6)/C6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="str">
+        <f>EEZ.Summary!A7</f>
+        <v>Puerto Rico + US V.I.</v>
+      </c>
+      <c r="B7" t="str">
+        <f>EPRI!B7</f>
+        <v>N/A</v>
+      </c>
+      <c r="C7">
+        <f>EPRI!C7</f>
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <f>Near.Summary!F7</f>
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <f>Near.Summary!G7</f>
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="G7" s="2">
+        <f>(F7-C7)/C7</f>
+        <v>-0.33333333333333331</v>
+      </c>
+      <c r="H7" s="2">
+        <f>(E7-F7)/C7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="str">
+        <f>EEZ.Summary!A8</f>
+        <v>TOTAL</v>
+      </c>
+      <c r="B8">
+        <f>SUM(B2:B5)</f>
+        <v>2100</v>
+      </c>
+      <c r="C8">
+        <f>EPRI!C8</f>
+        <v>2640</v>
+      </c>
+      <c r="D8">
+        <f>Near.Summary!F8</f>
+        <v>1850</v>
+      </c>
+      <c r="E8">
+        <f>Near.Summary!G8</f>
+        <v>1860</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>1855</v>
+      </c>
+      <c r="G8" s="2">
+        <f>(F8-C8)/C8</f>
+        <v>-0.29734848484848486</v>
+      </c>
+      <c r="H8" s="2">
+        <f>(E8-F8)/C8</f>
+        <v>1.893939393939394E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleanup the run_calc_spatial script.
</commit_message>
<xml_diff>
--- a/results/Total_Results.xlsx
+++ b/results/Total_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lkilcher/Dropbox/work/mhk/wave_res/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78BF8903-C50F-E84B-B862-361E300B7A45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8B6970-38B0-4A4C-B82C-E6FBD9D98489}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="16160" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="11060" windowWidth="28800" windowHeight="16160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EEZ.bl" sheetId="2" r:id="rId1"/>
@@ -135,12 +135,6 @@
     <t>Potential Local</t>
   </si>
   <si>
-    <t>Total 0</t>
-  </si>
-  <si>
-    <t>Total X</t>
-  </si>
-  <si>
     <t>Hawaii</t>
   </si>
   <si>
@@ -238,6 +232,12 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Remote+Natural</t>
+  </si>
+  <si>
+    <t>Remote+Potential</t>
   </si>
 </sst>
 </file>
@@ -1126,7 +1126,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1144,7 +1144,7 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -1215,7 +1215,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3">
         <v>30093.24609375</v>
@@ -1263,7 +1263,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B4">
         <v>493194.40625</v>
@@ -1311,7 +1311,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B5">
         <v>1471186.625</v>
@@ -1407,7 +1407,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7">
         <v>403368.46875</v>
@@ -1455,7 +1455,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B8">
         <v>318582.125</v>
@@ -1503,7 +1503,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B9">
         <v>1186728.875</v>
@@ -1813,13 +1813,13 @@
         <v>Region</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1993,7 +1993,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2011,7 +2011,7 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -2078,7 +2078,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3">
         <v>30093.24609375</v>
@@ -2122,7 +2122,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B4">
         <v>493194.40625</v>
@@ -2166,7 +2166,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B5">
         <v>1471186.625</v>
@@ -2254,7 +2254,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7">
         <v>403368.46875</v>
@@ -2298,7 +2298,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B8">
         <v>318582.125</v>
@@ -2342,7 +2342,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B9">
         <v>1186728.875</v>
@@ -2621,7 +2621,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2639,7 +2639,7 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -2706,7 +2706,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3">
         <v>258005.609375</v>
@@ -2750,7 +2750,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B4">
         <v>476253.3125</v>
@@ -2794,7 +2794,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B5">
         <v>1822151.625</v>
@@ -2882,7 +2882,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7">
         <v>805216.75</v>
@@ -2926,7 +2926,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B8">
         <v>665975.375</v>
@@ -2970,7 +2970,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B9">
         <v>1727482</v>
@@ -3242,14 +3242,14 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -3267,7 +3267,7 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -3334,7 +3334,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3">
         <v>258005.609375</v>
@@ -3378,7 +3378,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B4">
         <v>476253.3125</v>
@@ -3422,7 +3422,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B5">
         <v>1822151.625</v>
@@ -3510,7 +3510,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7">
         <v>805216.75</v>
@@ -3554,7 +3554,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B8">
         <v>665975.375</v>
@@ -3598,7 +3598,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B9">
         <v>1727482</v>
@@ -3932,7 +3932,7 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C6">
         <v>80</v>
@@ -3943,7 +3943,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C7">
         <v>30</v>
@@ -3967,8 +3967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3989,7 +3989,7 @@
         <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>22</v>
@@ -3998,10 +3998,10 @@
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -4035,7 +4035,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3" s="14">
         <f>EEZ.bl!C3</f>
@@ -4064,7 +4064,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" s="14">
         <f>EEZ.bl!C4</f>
@@ -4093,7 +4093,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B5" s="14">
         <f>EEZ.bl!C5</f>
@@ -4151,7 +4151,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B7" s="14">
         <f>EEZ.bl!C7</f>
@@ -4180,7 +4180,7 @@
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B8" s="14">
         <f>EEZ.bl!C8</f>
@@ -4209,7 +4209,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B9" s="14">
         <f>EEZ.bl!C9</f>
@@ -4238,7 +4238,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B10" s="13">
         <f>EEZ.bl!C10</f>
@@ -4267,7 +4267,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B11" s="13">
         <f>EEZ.bl!C11</f>
@@ -4296,7 +4296,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B12" s="13">
         <f>EEZ.bl!C12</f>
@@ -4325,7 +4325,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B13" s="13">
         <f>EEZ.bl!C13</f>
@@ -4354,7 +4354,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B14" s="15">
         <f>SUM(B2,B6,B10:B13)</f>
@@ -4401,28 +4401,28 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
         <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" t="s">
-        <v>32</v>
-      </c>
       <c r="I1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -4844,8 +4844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F893EFA9-E3BF-F249-9404-9C034DB18919}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4864,7 +4864,7 @@
         <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>22</v>
@@ -4873,10 +4873,10 @@
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -5107,8 +5107,7 @@
         <v>0.91787469215999995</v>
       </c>
       <c r="E9" s="14">
-        <f>Near.ex!N9</f>
-        <v>-1.8966801600000001</v>
+        <v>0</v>
       </c>
       <c r="F9" s="14">
         <f t="shared" si="0"/>
@@ -5116,7 +5115,7 @@
       </c>
       <c r="G9" s="14">
         <f t="shared" si="1"/>
-        <v>37.457175532800001</v>
+        <v>39.353855692800003</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -5291,28 +5290,28 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" t="s">
-        <v>45</v>
-      </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" t="s">
-        <v>32</v>
-      </c>
       <c r="I1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -5533,11 +5532,11 @@
       </c>
       <c r="F9">
         <f>Near.Summary!G9</f>
-        <v>37.457175532800001</v>
+        <v>39.353855692800003</v>
       </c>
       <c r="G9">
         <f t="shared" ref="G9:G16" si="4">AVERAGE(E9:F9)</f>
-        <v>38.864452958880001</v>
+        <v>39.812793038880002</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>

</xml_diff>

<commit_message>
Calculate technical resource using method in QTR
</commit_message>
<xml_diff>
--- a/results/Total_Results.xlsx
+++ b/results/Total_Results.xlsx
@@ -8,21 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lkilcher/Dropbox/work/mhk/wave_res/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8B6970-38B0-4A4C-B82C-E6FBD9D98489}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6EA1FA8-BBFE-7F4F-9B57-A83592E85894}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="11060" windowWidth="28800" windowHeight="16160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33760" yWindow="460" windowWidth="28800" windowHeight="16020" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EEZ.bl" sheetId="2" r:id="rId1"/>
     <sheet name="EEZ.ex" sheetId="1" r:id="rId2"/>
-    <sheet name="Near.bl" sheetId="7" r:id="rId3"/>
-    <sheet name="Near.ex" sheetId="8" r:id="rId4"/>
-    <sheet name="EPRI" sheetId="4" r:id="rId5"/>
-    <sheet name="EEZ.Summary" sheetId="3" r:id="rId6"/>
-    <sheet name="EEZ.COMPARE" sheetId="5" r:id="rId7"/>
-    <sheet name="Near.Summary" sheetId="9" r:id="rId8"/>
-    <sheet name="Near.COMPARE" sheetId="10" r:id="rId9"/>
-    <sheet name="one-way" sheetId="6" r:id="rId10"/>
+    <sheet name="EEZ.technical" sheetId="11" r:id="rId3"/>
+    <sheet name="Near.bl" sheetId="7" r:id="rId4"/>
+    <sheet name="Near.ex" sheetId="8" r:id="rId5"/>
+    <sheet name="near.technical" sheetId="12" r:id="rId6"/>
+    <sheet name="EPRI" sheetId="4" r:id="rId7"/>
+    <sheet name="EEZ.Summary" sheetId="3" r:id="rId8"/>
+    <sheet name="EEZ.COMPARE" sheetId="5" r:id="rId9"/>
+    <sheet name="QTR Table-4.N.2" sheetId="14" r:id="rId10"/>
+    <sheet name="Near.Summary" sheetId="9" r:id="rId11"/>
+    <sheet name="Near.COMPARE" sheetId="10" r:id="rId12"/>
+    <sheet name="one-way" sheetId="6" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -61,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="69">
   <si>
     <t>bdir</t>
   </si>
@@ -238,6 +241,36 @@
   </si>
   <si>
     <t>Remote+Potential</t>
+  </si>
+  <si>
+    <t>Extraction Factor (kW/m):</t>
+  </si>
+  <si>
+    <t>Theoretical - TOTAL US</t>
+  </si>
+  <si>
+    <t>Technical - TOTAL US</t>
+  </si>
+  <si>
+    <t>Technical - CONUS</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>CONUS</t>
+  </si>
+  <si>
+    <t>Technical Ranges: nearshore - EEZ</t>
+  </si>
+  <si>
+    <t>Technical Ranges: near (threshold 8000 - 1000)</t>
+  </si>
+  <si>
+    <t>WAVE ENERGY</t>
+  </si>
+  <si>
+    <t>Extraction Factor (kW/m)</t>
   </si>
 </sst>
 </file>
@@ -245,7 +278,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -743,7 +776,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -752,14 +785,22 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="16" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="16" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="16" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1795,6 +1836,996 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893C187D-BAAF-1F4C-A561-9DE5DDD64B38}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="2" max="7" width="11.83203125" customWidth="1"/>
+    <col min="8" max="8" width="51.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B1" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="17"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="16">
+        <f>EEZ.Summary!F$14</f>
+        <v>3271.4238489907202</v>
+      </c>
+      <c r="C2" s="16">
+        <f>EEZ.Summary!G$14</f>
+        <v>4089.1855900799997</v>
+      </c>
+      <c r="D2" s="16">
+        <f>near.technical!E14</f>
+        <v>867.40668682175999</v>
+      </c>
+      <c r="E2" s="16">
+        <f>EEZ.technical!E14</f>
+        <v>1040.9492832585599</v>
+      </c>
+      <c r="F2" s="16">
+        <f>near.technical!E15</f>
+        <v>265.87267497983999</v>
+      </c>
+      <c r="G2" s="16">
+        <f>EEZ.technical!E15</f>
+        <v>278.02642883807999</v>
+      </c>
+      <c r="H2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="19"/>
+      <c r="B3" s="16">
+        <f>EEZ.Summary!F$14</f>
+        <v>3271.4238489907202</v>
+      </c>
+      <c r="C3" s="16">
+        <f>EEZ.Summary!G$14</f>
+        <v>4089.1855900799997</v>
+      </c>
+      <c r="D3" s="16">
+        <f>near.technical!E14</f>
+        <v>867.40668682175999</v>
+      </c>
+      <c r="E3" s="16">
+        <f>near.technical!B14</f>
+        <v>1807.8990108662399</v>
+      </c>
+      <c r="F3" s="16">
+        <f>near.technical!E15</f>
+        <v>265.87267497983999</v>
+      </c>
+      <c r="G3" s="16">
+        <f>near.technical!B15</f>
+        <v>533.96275740672002</v>
+      </c>
+      <c r="H3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F893EFA9-E3BF-F249-9404-9C034DB18919}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="str">
+        <f>EEZ.Summary!A2</f>
+        <v>West Coast</v>
+      </c>
+      <c r="B2" s="13">
+        <f>Near.bl!C2</f>
+        <v>414.89609736192</v>
+      </c>
+      <c r="C2" s="8">
+        <f>Near.bl!C2/Near.bl!B2*1000000000/(365*24)</f>
+        <v>18.526980777148271</v>
+      </c>
+      <c r="D2" s="13">
+        <f>Near.bl!N2</f>
+        <v>0.36441943391999998</v>
+      </c>
+      <c r="E2" s="13">
+        <f>Near.ex!N2</f>
+        <v>2.00970896832</v>
+      </c>
+      <c r="F2" s="13">
+        <f>B2+D2</f>
+        <v>415.26051679583998</v>
+      </c>
+      <c r="G2" s="13">
+        <f>B2+E2</f>
+        <v>416.90580633024001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="str">
+        <f>EEZ.Summary!A3</f>
+        <v>Washington</v>
+      </c>
+      <c r="B3" s="14">
+        <f>Near.bl!C3</f>
+        <v>68.935845888000003</v>
+      </c>
+      <c r="C3" s="9">
+        <f>Near.bl!C3/Near.bl!B3*1000000000/(365*24)</f>
+        <v>30.500843834608972</v>
+      </c>
+      <c r="D3" s="14">
+        <f>Near.bl!N3</f>
+        <v>-0.18954558624000001</v>
+      </c>
+      <c r="E3" s="14">
+        <f>Near.ex!N3</f>
+        <v>5.5936077719999998E-2</v>
+      </c>
+      <c r="F3" s="14">
+        <f t="shared" ref="F3:F13" si="0">B3+D3</f>
+        <v>68.746300301760002</v>
+      </c>
+      <c r="G3" s="14">
+        <f t="shared" ref="G3:G13" si="1">B3+E3</f>
+        <v>68.991781965720008</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="str">
+        <f>EEZ.Summary!A4</f>
+        <v>Oregon</v>
+      </c>
+      <c r="B4" s="14">
+        <f>Near.bl!C4</f>
+        <v>128.66570489855999</v>
+      </c>
+      <c r="C4" s="9">
+        <f>Near.bl!C4/Near.bl!B4*1000000000/(365*24)</f>
+        <v>30.840448707640217</v>
+      </c>
+      <c r="D4" s="14">
+        <f>Near.bl!N4</f>
+        <v>8.8743801959999993E-2</v>
+      </c>
+      <c r="E4" s="14">
+        <f>Near.ex!N4</f>
+        <v>0.58485306047999996</v>
+      </c>
+      <c r="F4" s="14">
+        <f t="shared" si="0"/>
+        <v>128.75444870051999</v>
+      </c>
+      <c r="G4" s="14">
+        <f t="shared" si="1"/>
+        <v>129.25055795903998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="str">
+        <f>EEZ.Summary!A5</f>
+        <v>California</v>
+      </c>
+      <c r="B5" s="14">
+        <f>Near.bl!C5</f>
+        <v>218.28275306495999</v>
+      </c>
+      <c r="C5" s="9">
+        <f>Near.bl!C5/Near.bl!B5*1000000000/(365*24)</f>
+        <v>13.675109224788031</v>
+      </c>
+      <c r="D5" s="14">
+        <f>Near.bl!N5</f>
+        <v>0.45424419360000001</v>
+      </c>
+      <c r="E5" s="14">
+        <f>Near.ex!N5</f>
+        <v>1.3556570937600001</v>
+      </c>
+      <c r="F5" s="14">
+        <f t="shared" si="0"/>
+        <v>218.73699725856</v>
+      </c>
+      <c r="G5" s="14">
+        <f t="shared" si="1"/>
+        <v>219.63841015871998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="str">
+        <f>EEZ.Summary!A6</f>
+        <v>East Coast</v>
+      </c>
+      <c r="B6" s="13">
+        <f>Near.bl!C6</f>
+        <v>93.129650626559993</v>
+      </c>
+      <c r="C6" s="8">
+        <f>Near.bl!C6/Near.bl!B6*1000000000/(365*24)</f>
+        <v>3.323639053273399</v>
+      </c>
+      <c r="D6" s="13">
+        <f>Near.bl!N6</f>
+        <v>4.6155111283199997</v>
+      </c>
+      <c r="E6" s="13">
+        <f>Near.ex!N6</f>
+        <v>0.42721191984000001</v>
+      </c>
+      <c r="F6" s="13">
+        <f t="shared" si="0"/>
+        <v>97.745161754879987</v>
+      </c>
+      <c r="G6" s="13">
+        <f t="shared" si="1"/>
+        <v>93.556862546399998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="str">
+        <f>EEZ.Summary!A7</f>
+        <v>New England</v>
+      </c>
+      <c r="B7" s="14">
+        <f>Near.bl!C7</f>
+        <v>31.333705390079999</v>
+      </c>
+      <c r="C7" s="9">
+        <f>Near.bl!C7/Near.bl!B7*1000000000/(365*24)</f>
+        <v>4.4421666687882482</v>
+      </c>
+      <c r="D7" s="14">
+        <f>Near.bl!N7</f>
+        <v>2.76157892736</v>
+      </c>
+      <c r="E7" s="14">
+        <f>Near.ex!N7</f>
+        <v>2.6711488166400001</v>
+      </c>
+      <c r="F7" s="14">
+        <f t="shared" si="0"/>
+        <v>34.095284317439997</v>
+      </c>
+      <c r="G7" s="14">
+        <f t="shared" si="1"/>
+        <v>34.004854206719997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="str">
+        <f>EEZ.Summary!A8</f>
+        <v>Mid-Atlantic</v>
+      </c>
+      <c r="B8" s="14">
+        <f>Near.bl!C8</f>
+        <v>22.48827506688</v>
+      </c>
+      <c r="C8" s="9">
+        <f>Near.bl!C8/Near.bl!B8*1000000000/(365*24)</f>
+        <v>3.8547291452030032</v>
+      </c>
+      <c r="D8" s="14">
+        <f>Near.bl!N8</f>
+        <v>0.85168658496000005</v>
+      </c>
+      <c r="E8" s="14">
+        <f>Near.ex!N8</f>
+        <v>-0.38121943200000002</v>
+      </c>
+      <c r="F8" s="14">
+        <f t="shared" si="0"/>
+        <v>23.339961651839999</v>
+      </c>
+      <c r="G8" s="14">
+        <f t="shared" si="1"/>
+        <v>22.107055634879998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="str">
+        <f>EEZ.Summary!A9</f>
+        <v>Southeast</v>
+      </c>
+      <c r="B9" s="14">
+        <f>Near.bl!C9</f>
+        <v>39.353855692800003</v>
+      </c>
+      <c r="C9" s="9">
+        <f>Near.bl!C9/Near.bl!B9*1000000000/(365*24)</f>
+        <v>2.6005766080341215</v>
+      </c>
+      <c r="D9" s="14">
+        <f>Near.bl!N9</f>
+        <v>0.91787469215999995</v>
+      </c>
+      <c r="E9" s="14">
+        <v>0</v>
+      </c>
+      <c r="F9" s="14">
+        <f t="shared" si="0"/>
+        <v>40.271730384960001</v>
+      </c>
+      <c r="G9" s="14">
+        <f t="shared" si="1"/>
+        <v>39.353855692800003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="str">
+        <f>EEZ.Summary!A10</f>
+        <v>Hawaii</v>
+      </c>
+      <c r="B10" s="13">
+        <f>Near.bl!C10</f>
+        <v>117.97534961664</v>
+      </c>
+      <c r="C10" s="8">
+        <f>Near.bl!C10/Near.bl!B10*1000000000/(365*24)</f>
+        <v>7.6960863847117249</v>
+      </c>
+      <c r="D10" s="13">
+        <f>Near.bl!N10</f>
+        <v>0.56034587424000004</v>
+      </c>
+      <c r="E10" s="13">
+        <f>Near.ex!N10</f>
+        <v>1.17849569472</v>
+      </c>
+      <c r="F10" s="13">
+        <f t="shared" si="0"/>
+        <v>118.53569549088</v>
+      </c>
+      <c r="G10" s="13">
+        <f t="shared" si="1"/>
+        <v>119.15384531136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="str">
+        <f>EEZ.Summary!A11</f>
+        <v>Alaska</v>
+      </c>
+      <c r="B11" s="13">
+        <f>Near.bl!C11</f>
+        <v>1135.2602984447999</v>
+      </c>
+      <c r="C11" s="8">
+        <f>Near.bl!C11/Near.bl!B11*1000000000/(365*24)</f>
+        <v>11.5652459213601</v>
+      </c>
+      <c r="D11" s="13">
+        <f>Near.bl!N11</f>
+        <v>54.088896675839997</v>
+      </c>
+      <c r="E11" s="13">
+        <f>Near.ex!N11</f>
+        <v>59.108472545280001</v>
+      </c>
+      <c r="F11" s="13">
+        <f t="shared" si="0"/>
+        <v>1189.3491951206399</v>
+      </c>
+      <c r="G11" s="13">
+        <f t="shared" si="1"/>
+        <v>1194.3687709900798</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="str">
+        <f>EEZ.Summary!A12</f>
+        <v>Gulf of Mexico</v>
+      </c>
+      <c r="B12" s="13">
+        <f>Near.bl!C12</f>
+        <v>24.46945572864</v>
+      </c>
+      <c r="C12" s="8">
+        <f>Near.bl!C12/Near.bl!B12*1000000000/(365*24)</f>
+        <v>1.0255056371630749</v>
+      </c>
+      <c r="D12" s="13">
+        <f>Near.bl!N12</f>
+        <v>2.48532721152</v>
+      </c>
+      <c r="E12" s="13">
+        <f>Near.ex!N12</f>
+        <v>-0.29779224048000003</v>
+      </c>
+      <c r="F12" s="13">
+        <f t="shared" si="0"/>
+        <v>26.954782940160001</v>
+      </c>
+      <c r="G12" s="13">
+        <f t="shared" si="1"/>
+        <v>24.17166348816</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="str">
+        <f>EEZ.Summary!A13</f>
+        <v>Puerto Rico + US V.I.</v>
+      </c>
+      <c r="B13" s="13">
+        <f>Near.bl!C13</f>
+        <v>17.640082360320001</v>
+      </c>
+      <c r="C13" s="8">
+        <f>Near.bl!C13/Near.bl!B13*1000000000/(365*24)</f>
+        <v>3.1644058514638971</v>
+      </c>
+      <c r="D13" s="13">
+        <f>Near.bl!N13</f>
+        <v>0.21637522368000001</v>
+      </c>
+      <c r="E13" s="13">
+        <f>Near.ex!N13</f>
+        <v>0.36620079744</v>
+      </c>
+      <c r="F13" s="13">
+        <f t="shared" si="0"/>
+        <v>17.856457584000001</v>
+      </c>
+      <c r="G13" s="13">
+        <f t="shared" si="1"/>
+        <v>18.006283157760002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="str">
+        <f>EEZ.Summary!A14</f>
+        <v>Total</v>
+      </c>
+      <c r="B14" s="15">
+        <f>SUM(B2,B6,B10:B13)</f>
+        <v>1803.3709341388799</v>
+      </c>
+      <c r="C14" s="12">
+        <f>Near.bl!C14/Near.bl!B14*1000000000/(365*24)</f>
+        <v>9.3274321180344764</v>
+      </c>
+      <c r="D14" s="15">
+        <f>SUM(D2,D6,D10:D13)</f>
+        <v>62.330875547519994</v>
+      </c>
+      <c r="E14" s="15">
+        <f t="shared" ref="E14:G14" si="2">SUM(E2,E6,E10:E13)</f>
+        <v>62.792297685120005</v>
+      </c>
+      <c r="F14" s="15">
+        <f t="shared" si="2"/>
+        <v>1865.7018096863999</v>
+      </c>
+      <c r="G14" s="15">
+        <f t="shared" si="2"/>
+        <v>1866.1632318239997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FFF2529-D61C-C04A-AE20-738CA7021AB0}">
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" customWidth="1"/>
+    <col min="7" max="7" width="9.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>EEZ.Summary!A2</f>
+        <v>West Coast</v>
+      </c>
+      <c r="B2">
+        <f>EPRI!B2</f>
+        <v>440</v>
+      </c>
+      <c r="C2">
+        <f>EPRI!C2</f>
+        <v>590</v>
+      </c>
+      <c r="D2">
+        <v>419</v>
+      </c>
+      <c r="E2">
+        <f>Near.Summary!F2</f>
+        <v>415.26051679583998</v>
+      </c>
+      <c r="F2">
+        <f>Near.Summary!G2</f>
+        <v>416.90580633024001</v>
+      </c>
+      <c r="G2">
+        <f>AVERAGE(E2:F2)</f>
+        <v>416.08316156303999</v>
+      </c>
+      <c r="H2" s="2">
+        <f t="shared" ref="H2:H14" si="0">(G2-C2)/C2</f>
+        <v>-0.29477430243552544</v>
+      </c>
+      <c r="I2" s="2">
+        <f t="shared" ref="I2:I14" si="1">(F2-G2)/C2</f>
+        <v>1.3943131647457926E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f>EEZ.Summary!A3</f>
+        <v>Washington</v>
+      </c>
+      <c r="B3">
+        <f>EPRI!B3</f>
+        <v>110</v>
+      </c>
+      <c r="D3">
+        <v>172</v>
+      </c>
+      <c r="E3">
+        <f>Near.Summary!F3</f>
+        <v>68.746300301760002</v>
+      </c>
+      <c r="F3">
+        <f>Near.Summary!G3</f>
+        <v>68.991781965720008</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G8" si="2">AVERAGE(E3:F3)</f>
+        <v>68.869041133740012</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f>EEZ.Summary!A4</f>
+        <v>Oregon</v>
+      </c>
+      <c r="B4">
+        <f>EPRI!B4</f>
+        <v>300</v>
+      </c>
+      <c r="D4">
+        <v>110</v>
+      </c>
+      <c r="E4">
+        <f>Near.Summary!F4</f>
+        <v>128.75444870051999</v>
+      </c>
+      <c r="F4">
+        <f>Near.Summary!G4</f>
+        <v>129.25055795903998</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>129.00250332977998</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="str">
+        <f>EEZ.Summary!A5</f>
+        <v>California</v>
+      </c>
+      <c r="B5">
+        <f>EPRI!B5</f>
+        <v>1250</v>
+      </c>
+      <c r="D5">
+        <v>803</v>
+      </c>
+      <c r="E5">
+        <f>Near.Summary!F5</f>
+        <v>218.73699725856</v>
+      </c>
+      <c r="F5">
+        <f>Near.Summary!G5</f>
+        <v>219.63841015871998</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>219.18770370863999</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="str">
+        <f>EEZ.Summary!A6</f>
+        <v>East Coast</v>
+      </c>
+      <c r="B6" t="str">
+        <f>EPRI!B6</f>
+        <v>N/A</v>
+      </c>
+      <c r="C6">
+        <f>EPRI!C3</f>
+        <v>240</v>
+      </c>
+      <c r="D6">
+        <v>60</v>
+      </c>
+      <c r="E6">
+        <f>Near.Summary!F6</f>
+        <v>97.745161754879987</v>
+      </c>
+      <c r="F6">
+        <f>Near.Summary!G6</f>
+        <v>93.556862546399998</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>95.651012150639986</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.60145411603900001</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="1"/>
+        <v>-8.7256233509999479E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="str">
+        <f>EEZ.Summary!A7</f>
+        <v>New England</v>
+      </c>
+      <c r="B7" t="str">
+        <f>EPRI!B7</f>
+        <v>N/A</v>
+      </c>
+      <c r="E7">
+        <f>Near.Summary!F7</f>
+        <v>34.095284317439997</v>
+      </c>
+      <c r="F7">
+        <f>Near.Summary!G7</f>
+        <v>34.004854206719997</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>34.050069262080001</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="str">
+        <f>EEZ.Summary!A8</f>
+        <v>Mid-Atlantic</v>
+      </c>
+      <c r="D8">
+        <f>SUM(D2:D7)</f>
+        <v>1564</v>
+      </c>
+      <c r="E8">
+        <f>Near.Summary!F8</f>
+        <v>23.339961651839999</v>
+      </c>
+      <c r="F8">
+        <f>Near.Summary!G8</f>
+        <v>22.107055634879998</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>22.723508643359999</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="str">
+        <f>EEZ.Summary!A9</f>
+        <v>Southeast</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ref="D9:D14" si="3">SUM(D3:D8)</f>
+        <v>2709</v>
+      </c>
+      <c r="E9">
+        <f>Near.Summary!F9</f>
+        <v>40.271730384960001</v>
+      </c>
+      <c r="F9">
+        <f>Near.Summary!G9</f>
+        <v>39.353855692800003</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ref="G9:G14" si="4">AVERAGE(E9:F9)</f>
+        <v>39.812793038880002</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="str">
+        <f>EEZ.Summary!A10</f>
+        <v>Hawaii</v>
+      </c>
+      <c r="C10">
+        <f>EPRI!C4</f>
+        <v>130</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="3"/>
+        <v>5246</v>
+      </c>
+      <c r="E10">
+        <f>Near.Summary!F10</f>
+        <v>118.53569549088</v>
+      </c>
+      <c r="F10">
+        <f>Near.Summary!G10</f>
+        <v>119.15384531136</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="4"/>
+        <v>118.84477040112</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="0"/>
+        <v>-8.5809458452923065E-2</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="1"/>
+        <v>2.377499309538459E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="str">
+        <f>EEZ.Summary!A11</f>
+        <v>Alaska</v>
+      </c>
+      <c r="C11">
+        <f>EPRI!C5</f>
+        <v>1570</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="3"/>
+        <v>10382</v>
+      </c>
+      <c r="E11">
+        <f>Near.Summary!F11</f>
+        <v>1189.3491951206399</v>
+      </c>
+      <c r="F11">
+        <f>Near.Summary!G11</f>
+        <v>1194.3687709900798</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="4"/>
+        <v>1191.8589830553599</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.24085415092015294</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="1"/>
+        <v>1.5985910412228996E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="str">
+        <f>EEZ.Summary!A12</f>
+        <v>Gulf of Mexico</v>
+      </c>
+      <c r="C12">
+        <f>EPRI!C6</f>
+        <v>80</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="3"/>
+        <v>19961</v>
+      </c>
+      <c r="E12">
+        <f>Near.Summary!F12</f>
+        <v>26.954782940160001</v>
+      </c>
+      <c r="F12">
+        <f>Near.Summary!G12</f>
+        <v>24.17166348816</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="4"/>
+        <v>25.563223214160001</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.68045970982299997</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="1"/>
+        <v>-1.7394496575000008E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="str">
+        <f>EEZ.Summary!A13</f>
+        <v>Puerto Rico + US V.I.</v>
+      </c>
+      <c r="C13">
+        <f>EPRI!C7</f>
+        <v>30</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="3"/>
+        <v>39862</v>
+      </c>
+      <c r="E13">
+        <f>Near.Summary!F13</f>
+        <v>17.856457584000001</v>
+      </c>
+      <c r="F13">
+        <f>Near.Summary!G13</f>
+        <v>18.006283157760002</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="4"/>
+        <v>17.931370370880003</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.40228765430399988</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="1"/>
+        <v>2.4970928959999602E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="str">
+        <f>EEZ.Summary!A14</f>
+        <v>Total</v>
+      </c>
+      <c r="B14">
+        <f>SUM(B2:B5)</f>
+        <v>2100</v>
+      </c>
+      <c r="C14">
+        <f>EPRI!C8</f>
+        <v>2640</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="3"/>
+        <v>79724</v>
+      </c>
+      <c r="E14">
+        <f>Near.Summary!F14</f>
+        <v>1865.7018096863999</v>
+      </c>
+      <c r="F14">
+        <f>Near.Summary!G14</f>
+        <v>1866.1632318239997</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="4"/>
+        <v>1865.9325207551997</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.29320737850181833</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="1"/>
+        <v>8.7390556363643688E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -2610,6 +3641,285 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{356F04A3-FC2C-4542-8490-87ECB75F1C7E}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="1">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="16">
+        <v>417.03496138752001</v>
+      </c>
+      <c r="C2" s="16">
+        <v>399.56333789183998</v>
+      </c>
+      <c r="D2" s="16">
+        <v>329.67702331392002</v>
+      </c>
+      <c r="E2" s="16">
+        <v>277.71025219583998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="16">
+        <v>9.6699916031999997</v>
+      </c>
+      <c r="C3" s="16">
+        <v>9.4063753113599997</v>
+      </c>
+      <c r="D3" s="16">
+        <v>8.3519073408000004</v>
+      </c>
+      <c r="E3" s="16">
+        <v>7.5610567833599998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="16">
+        <v>157.84685543424001</v>
+      </c>
+      <c r="C4" s="16">
+        <v>153.5264649216</v>
+      </c>
+      <c r="D4" s="16">
+        <v>136.24492978175999</v>
+      </c>
+      <c r="E4" s="16">
+        <v>123.2837941248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="16">
+        <v>249.51813341184001</v>
+      </c>
+      <c r="C5" s="16">
+        <v>236.63053578239999</v>
+      </c>
+      <c r="D5" s="16">
+        <v>185.08014526464001</v>
+      </c>
+      <c r="E5" s="16">
+        <v>146.86542483456</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="16">
+        <v>106.30601822208</v>
+      </c>
+      <c r="C6" s="16">
+        <v>89.585993195520004</v>
+      </c>
+      <c r="D6" s="16">
+        <v>24.035778263040001</v>
+      </c>
+      <c r="E6" s="16">
+        <v>0.31617664224000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="16">
+        <v>26.454903982080001</v>
+      </c>
+      <c r="C7" s="16">
+        <v>22.92139413504</v>
+      </c>
+      <c r="D7" s="16">
+        <v>8.7873637171199999</v>
+      </c>
+      <c r="E7" s="16">
+        <v>2.1120219839999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="16">
+        <v>20.4428069376</v>
+      </c>
+      <c r="C8" s="16">
+        <v>17.652029598719999</v>
+      </c>
+      <c r="D8" s="16">
+        <v>6.4889112729600003</v>
+      </c>
+      <c r="E8" s="16">
+        <v>0.29505642240000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="16">
+        <v>59.408320757760002</v>
+      </c>
+      <c r="C9" s="16">
+        <v>49.012575068159997</v>
+      </c>
+      <c r="D9" s="16">
+        <v>8.7595060761599992</v>
+      </c>
+      <c r="E9" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="16">
+        <v>368.65472544767999</v>
+      </c>
+      <c r="C10" s="16">
+        <v>330.51132739584</v>
+      </c>
+      <c r="D10" s="16">
+        <v>191.27497506815999</v>
+      </c>
+      <c r="E10" s="16">
+        <v>109.74450855936</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="16">
+        <v>1041.5315075481601</v>
+      </c>
+      <c r="C11" s="16">
+        <v>992.96993820672003</v>
+      </c>
+      <c r="D11" s="16">
+        <v>798.72392097791999</v>
+      </c>
+      <c r="E11" s="16">
+        <v>653.17834586111996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="16">
+        <v>12.89082579456</v>
+      </c>
+      <c r="C12" s="16">
+        <v>4.8840075110400001</v>
+      </c>
+      <c r="D12" s="16">
+        <v>0</v>
+      </c>
+      <c r="E12" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="16">
+        <v>5.8012246425600003</v>
+      </c>
+      <c r="C13" s="16">
+        <v>4.9069752499200003</v>
+      </c>
+      <c r="D13" s="16">
+        <v>1.32997767936</v>
+      </c>
+      <c r="E13" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="18">
+        <f>SUM(B2,B6,B10,B11,B12,B13)</f>
+        <v>1952.2192630425602</v>
+      </c>
+      <c r="C14" s="18">
+        <f t="shared" ref="C14:E14" si="0">SUM(C2,C6,C10,C11,C12,C13)</f>
+        <v>1822.4215794508798</v>
+      </c>
+      <c r="D14" s="18">
+        <f t="shared" si="0"/>
+        <v>1345.0416753023999</v>
+      </c>
+      <c r="E14" s="18">
+        <f t="shared" si="0"/>
+        <v>1040.9492832585599</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="18">
+        <f>SUM(B2,B6,B12)</f>
+        <v>536.23180540416001</v>
+      </c>
+      <c r="C15" s="18">
+        <f t="shared" ref="C15:E15" si="1">SUM(C2,C6,C12)</f>
+        <v>494.03333859840001</v>
+      </c>
+      <c r="D15" s="18">
+        <f t="shared" si="1"/>
+        <v>353.71280157696003</v>
+      </c>
+      <c r="E15" s="18">
+        <f t="shared" si="1"/>
+        <v>278.02642883807999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51B6B5B9-50BB-3A4E-98D2-F24B327EABE8}">
   <dimension ref="A1:N14"/>
   <sheetViews>
@@ -3237,7 +4547,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F8BC87F-C28B-3641-A3EB-72C101404CE7}">
   <dimension ref="A1:N14"/>
   <sheetViews>
@@ -3865,7 +5175,288 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83D0FE4B-FC5C-C341-B515-8969CD7528FD}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>5</v>
+      </c>
+      <c r="E1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>416.16007593984</v>
+      </c>
+      <c r="C2">
+        <v>394.43006423039998</v>
+      </c>
+      <c r="D2">
+        <v>316.08140464128002</v>
+      </c>
+      <c r="E2">
+        <v>265.87267497983999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3">
+        <v>68.940008079359998</v>
+      </c>
+      <c r="C3">
+        <v>66.679870894079997</v>
+      </c>
+      <c r="D3">
+        <v>57.639353548800003</v>
+      </c>
+      <c r="E3">
+        <v>50.858968903680001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4">
+        <v>128.71922135040001</v>
+      </c>
+      <c r="C4">
+        <v>124.54724345856</v>
+      </c>
+      <c r="D4">
+        <v>107.8593318912</v>
+      </c>
+      <c r="E4">
+        <v>95.343398215679997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5">
+        <v>218.50085548032001</v>
+      </c>
+      <c r="C5">
+        <v>203.2029364224</v>
+      </c>
+      <c r="D5">
+        <v>150.58271920128001</v>
+      </c>
+      <c r="E5">
+        <v>119.67030337536001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>93.279884206079998</v>
+      </c>
+      <c r="C6">
+        <v>65.337541754879993</v>
+      </c>
+      <c r="D6">
+        <v>2.5341160665600002</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7">
+        <v>31.332826306560001</v>
+      </c>
+      <c r="C7">
+        <v>24.279127418880002</v>
+      </c>
+      <c r="D7">
+        <v>1.2534424704</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8">
+        <v>22.466746490879999</v>
+      </c>
+      <c r="C8">
+        <v>16.63279953408</v>
+      </c>
+      <c r="D8">
+        <v>0.39242914847999999</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9">
+        <v>39.480309166079998</v>
+      </c>
+      <c r="C9">
+        <v>24.425611438080001</v>
+      </c>
+      <c r="D9">
+        <v>0.88824437759999997</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>118.27432323072</v>
+      </c>
+      <c r="C10">
+        <v>102.9542252544</v>
+      </c>
+      <c r="D10">
+        <v>54.840301163520003</v>
+      </c>
+      <c r="E10">
+        <v>31.03552676352</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>1137.97040634528</v>
+      </c>
+      <c r="C11">
+        <v>1045.82996603424</v>
+      </c>
+      <c r="D11">
+        <v>752.99074399487995</v>
+      </c>
+      <c r="E11">
+        <v>570.49848507839999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>24.522797260800001</v>
+      </c>
+      <c r="C12">
+        <v>8.3624669952000001</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>17.691523883519999</v>
+      </c>
+      <c r="C13">
+        <v>12.68265287424</v>
+      </c>
+      <c r="D13">
+        <v>2.1331920307200001</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="1">
+        <f>SUM(B2,B6,B10:B13)</f>
+        <v>1807.8990108662399</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" ref="C14:E14" si="0">SUM(C2,C6,C10:C13)</f>
+        <v>1629.5969171433599</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>1128.57975789696</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="0"/>
+        <v>867.40668682175999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="1">
+        <f>SUM(B2,B6,B12)</f>
+        <v>533.96275740672002</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" ref="C15:E15" si="1">SUM(C2,C6,C12)</f>
+        <v>468.13007298047995</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="1"/>
+        <v>318.61552070784001</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="1"/>
+        <v>265.87267497983999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -3963,12 +5554,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4365,7 +5956,7 @@
         <v>14.996700460691404</v>
       </c>
       <c r="D14" s="15">
-        <f t="shared" ref="C14:G14" si="4">SUM(D2,D6,D10:D13)</f>
+        <f t="shared" ref="D14:G14" si="4">SUM(D2,D6,D10:D13)</f>
         <v>1324.8882034560002</v>
       </c>
       <c r="E14" s="15">
@@ -4386,7 +5977,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
@@ -4569,7 +6160,7 @@
         <v>0.30039876147200012</v>
       </c>
       <c r="I6" s="2">
-        <f t="shared" ref="I3:I14" si="2">(F6-G6)/C6</f>
+        <f t="shared" ref="I6:I14" si="2">(F6-G6)/C6</f>
         <v>0.12067992780800006</v>
       </c>
     </row>
@@ -4838,892 +6429,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F893EFA9-E3BF-F249-9404-9C034DB18919}">
-  <dimension ref="A1:G14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.1640625" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="str">
-        <f>EEZ.Summary!A2</f>
-        <v>West Coast</v>
-      </c>
-      <c r="B2" s="13">
-        <f>Near.bl!C2</f>
-        <v>414.89609736192</v>
-      </c>
-      <c r="C2" s="8">
-        <f>Near.bl!C2/Near.bl!B2*1000000000/(365*24)</f>
-        <v>18.526980777148271</v>
-      </c>
-      <c r="D2" s="13">
-        <f>Near.bl!N2</f>
-        <v>0.36441943391999998</v>
-      </c>
-      <c r="E2" s="13">
-        <f>Near.ex!N2</f>
-        <v>2.00970896832</v>
-      </c>
-      <c r="F2" s="13">
-        <f>B2+D2</f>
-        <v>415.26051679583998</v>
-      </c>
-      <c r="G2" s="13">
-        <f>B2+E2</f>
-        <v>416.90580633024001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="str">
-        <f>EEZ.Summary!A3</f>
-        <v>Washington</v>
-      </c>
-      <c r="B3" s="14">
-        <f>Near.bl!C3</f>
-        <v>68.935845888000003</v>
-      </c>
-      <c r="C3" s="9">
-        <f>Near.bl!C3/Near.bl!B3*1000000000/(365*24)</f>
-        <v>30.500843834608972</v>
-      </c>
-      <c r="D3" s="14">
-        <f>Near.bl!N3</f>
-        <v>-0.18954558624000001</v>
-      </c>
-      <c r="E3" s="14">
-        <f>Near.ex!N3</f>
-        <v>5.5936077719999998E-2</v>
-      </c>
-      <c r="F3" s="14">
-        <f t="shared" ref="F3:F13" si="0">B3+D3</f>
-        <v>68.746300301760002</v>
-      </c>
-      <c r="G3" s="14">
-        <f t="shared" ref="G3:G13" si="1">B3+E3</f>
-        <v>68.991781965720008</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="str">
-        <f>EEZ.Summary!A4</f>
-        <v>Oregon</v>
-      </c>
-      <c r="B4" s="14">
-        <f>Near.bl!C4</f>
-        <v>128.66570489855999</v>
-      </c>
-      <c r="C4" s="9">
-        <f>Near.bl!C4/Near.bl!B4*1000000000/(365*24)</f>
-        <v>30.840448707640217</v>
-      </c>
-      <c r="D4" s="14">
-        <f>Near.bl!N4</f>
-        <v>8.8743801959999993E-2</v>
-      </c>
-      <c r="E4" s="14">
-        <f>Near.ex!N4</f>
-        <v>0.58485306047999996</v>
-      </c>
-      <c r="F4" s="14">
-        <f t="shared" si="0"/>
-        <v>128.75444870051999</v>
-      </c>
-      <c r="G4" s="14">
-        <f t="shared" si="1"/>
-        <v>129.25055795903998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="str">
-        <f>EEZ.Summary!A5</f>
-        <v>California</v>
-      </c>
-      <c r="B5" s="14">
-        <f>Near.bl!C5</f>
-        <v>218.28275306495999</v>
-      </c>
-      <c r="C5" s="9">
-        <f>Near.bl!C5/Near.bl!B5*1000000000/(365*24)</f>
-        <v>13.675109224788031</v>
-      </c>
-      <c r="D5" s="14">
-        <f>Near.bl!N5</f>
-        <v>0.45424419360000001</v>
-      </c>
-      <c r="E5" s="14">
-        <f>Near.ex!N5</f>
-        <v>1.3556570937600001</v>
-      </c>
-      <c r="F5" s="14">
-        <f t="shared" si="0"/>
-        <v>218.73699725856</v>
-      </c>
-      <c r="G5" s="14">
-        <f t="shared" si="1"/>
-        <v>219.63841015871998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="str">
-        <f>EEZ.Summary!A6</f>
-        <v>East Coast</v>
-      </c>
-      <c r="B6" s="13">
-        <f>Near.bl!C6</f>
-        <v>93.129650626559993</v>
-      </c>
-      <c r="C6" s="8">
-        <f>Near.bl!C6/Near.bl!B6*1000000000/(365*24)</f>
-        <v>3.323639053273399</v>
-      </c>
-      <c r="D6" s="13">
-        <f>Near.bl!N6</f>
-        <v>4.6155111283199997</v>
-      </c>
-      <c r="E6" s="13">
-        <f>Near.ex!N6</f>
-        <v>0.42721191984000001</v>
-      </c>
-      <c r="F6" s="13">
-        <f t="shared" si="0"/>
-        <v>97.745161754879987</v>
-      </c>
-      <c r="G6" s="13">
-        <f t="shared" si="1"/>
-        <v>93.556862546399998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="str">
-        <f>EEZ.Summary!A7</f>
-        <v>New England</v>
-      </c>
-      <c r="B7" s="14">
-        <f>Near.bl!C7</f>
-        <v>31.333705390079999</v>
-      </c>
-      <c r="C7" s="9">
-        <f>Near.bl!C7/Near.bl!B7*1000000000/(365*24)</f>
-        <v>4.4421666687882482</v>
-      </c>
-      <c r="D7" s="14">
-        <f>Near.bl!N7</f>
-        <v>2.76157892736</v>
-      </c>
-      <c r="E7" s="14">
-        <f>Near.ex!N7</f>
-        <v>2.6711488166400001</v>
-      </c>
-      <c r="F7" s="14">
-        <f t="shared" si="0"/>
-        <v>34.095284317439997</v>
-      </c>
-      <c r="G7" s="14">
-        <f t="shared" si="1"/>
-        <v>34.004854206719997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="str">
-        <f>EEZ.Summary!A8</f>
-        <v>Mid-Atlantic</v>
-      </c>
-      <c r="B8" s="14">
-        <f>Near.bl!C8</f>
-        <v>22.48827506688</v>
-      </c>
-      <c r="C8" s="9">
-        <f>Near.bl!C8/Near.bl!B8*1000000000/(365*24)</f>
-        <v>3.8547291452030032</v>
-      </c>
-      <c r="D8" s="14">
-        <f>Near.bl!N8</f>
-        <v>0.85168658496000005</v>
-      </c>
-      <c r="E8" s="14">
-        <f>Near.ex!N8</f>
-        <v>-0.38121943200000002</v>
-      </c>
-      <c r="F8" s="14">
-        <f t="shared" si="0"/>
-        <v>23.339961651839999</v>
-      </c>
-      <c r="G8" s="14">
-        <f t="shared" si="1"/>
-        <v>22.107055634879998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="str">
-        <f>EEZ.Summary!A9</f>
-        <v>Southeast</v>
-      </c>
-      <c r="B9" s="14">
-        <f>Near.bl!C9</f>
-        <v>39.353855692800003</v>
-      </c>
-      <c r="C9" s="9">
-        <f>Near.bl!C9/Near.bl!B9*1000000000/(365*24)</f>
-        <v>2.6005766080341215</v>
-      </c>
-      <c r="D9" s="14">
-        <f>Near.bl!N9</f>
-        <v>0.91787469215999995</v>
-      </c>
-      <c r="E9" s="14">
-        <v>0</v>
-      </c>
-      <c r="F9" s="14">
-        <f t="shared" si="0"/>
-        <v>40.271730384960001</v>
-      </c>
-      <c r="G9" s="14">
-        <f t="shared" si="1"/>
-        <v>39.353855692800003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="str">
-        <f>EEZ.Summary!A10</f>
-        <v>Hawaii</v>
-      </c>
-      <c r="B10" s="13">
-        <f>Near.bl!C10</f>
-        <v>117.97534961664</v>
-      </c>
-      <c r="C10" s="8">
-        <f>Near.bl!C10/Near.bl!B10*1000000000/(365*24)</f>
-        <v>7.6960863847117249</v>
-      </c>
-      <c r="D10" s="13">
-        <f>Near.bl!N10</f>
-        <v>0.56034587424000004</v>
-      </c>
-      <c r="E10" s="13">
-        <f>Near.ex!N10</f>
-        <v>1.17849569472</v>
-      </c>
-      <c r="F10" s="13">
-        <f t="shared" si="0"/>
-        <v>118.53569549088</v>
-      </c>
-      <c r="G10" s="13">
-        <f t="shared" si="1"/>
-        <v>119.15384531136</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="str">
-        <f>EEZ.Summary!A11</f>
-        <v>Alaska</v>
-      </c>
-      <c r="B11" s="13">
-        <f>Near.bl!C11</f>
-        <v>1135.2602984447999</v>
-      </c>
-      <c r="C11" s="8">
-        <f>Near.bl!C11/Near.bl!B11*1000000000/(365*24)</f>
-        <v>11.5652459213601</v>
-      </c>
-      <c r="D11" s="13">
-        <f>Near.bl!N11</f>
-        <v>54.088896675839997</v>
-      </c>
-      <c r="E11" s="13">
-        <f>Near.ex!N11</f>
-        <v>59.108472545280001</v>
-      </c>
-      <c r="F11" s="13">
-        <f t="shared" si="0"/>
-        <v>1189.3491951206399</v>
-      </c>
-      <c r="G11" s="13">
-        <f t="shared" si="1"/>
-        <v>1194.3687709900798</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="str">
-        <f>EEZ.Summary!A12</f>
-        <v>Gulf of Mexico</v>
-      </c>
-      <c r="B12" s="13">
-        <f>Near.bl!C12</f>
-        <v>24.46945572864</v>
-      </c>
-      <c r="C12" s="8">
-        <f>Near.bl!C12/Near.bl!B12*1000000000/(365*24)</f>
-        <v>1.0255056371630749</v>
-      </c>
-      <c r="D12" s="13">
-        <f>Near.bl!N12</f>
-        <v>2.48532721152</v>
-      </c>
-      <c r="E12" s="13">
-        <f>Near.ex!N12</f>
-        <v>-0.29779224048000003</v>
-      </c>
-      <c r="F12" s="13">
-        <f t="shared" si="0"/>
-        <v>26.954782940160001</v>
-      </c>
-      <c r="G12" s="13">
-        <f t="shared" si="1"/>
-        <v>24.17166348816</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="str">
-        <f>EEZ.Summary!A13</f>
-        <v>Puerto Rico + US V.I.</v>
-      </c>
-      <c r="B13" s="13">
-        <f>Near.bl!C13</f>
-        <v>17.640082360320001</v>
-      </c>
-      <c r="C13" s="8">
-        <f>Near.bl!C13/Near.bl!B13*1000000000/(365*24)</f>
-        <v>3.1644058514638971</v>
-      </c>
-      <c r="D13" s="13">
-        <f>Near.bl!N13</f>
-        <v>0.21637522368000001</v>
-      </c>
-      <c r="E13" s="13">
-        <f>Near.ex!N13</f>
-        <v>0.36620079744</v>
-      </c>
-      <c r="F13" s="13">
-        <f t="shared" si="0"/>
-        <v>17.856457584000001</v>
-      </c>
-      <c r="G13" s="13">
-        <f t="shared" si="1"/>
-        <v>18.006283157760002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="str">
-        <f>EEZ.Summary!A14</f>
-        <v>Total</v>
-      </c>
-      <c r="B14" s="15">
-        <f>SUM(B2,B6,B10:B13)</f>
-        <v>1803.3709341388799</v>
-      </c>
-      <c r="C14" s="12">
-        <f>Near.bl!C14/Near.bl!B14*1000000000/(365*24)</f>
-        <v>9.3274321180344764</v>
-      </c>
-      <c r="D14" s="15">
-        <f>SUM(D2,D6,D10:D13)</f>
-        <v>62.330875547519994</v>
-      </c>
-      <c r="E14" s="15">
-        <f t="shared" ref="E14:G14" si="2">SUM(E2,E6,E10:E13)</f>
-        <v>62.792297685120005</v>
-      </c>
-      <c r="F14" s="15">
-        <f t="shared" si="2"/>
-        <v>1865.7018096863999</v>
-      </c>
-      <c r="G14" s="15">
-        <f t="shared" si="2"/>
-        <v>1866.1632318239997</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FFF2529-D61C-C04A-AE20-738CA7021AB0}">
-  <dimension ref="A1:I16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="16.83203125" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" customWidth="1"/>
-    <col min="7" max="7" width="9.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="str">
-        <f>EEZ.Summary!A2</f>
-        <v>West Coast</v>
-      </c>
-      <c r="B2">
-        <f>EPRI!B2</f>
-        <v>440</v>
-      </c>
-      <c r="C2">
-        <f>EPRI!C2</f>
-        <v>590</v>
-      </c>
-      <c r="D2">
-        <v>419</v>
-      </c>
-      <c r="E2">
-        <f>Near.Summary!F2</f>
-        <v>415.26051679583998</v>
-      </c>
-      <c r="F2">
-        <f>Near.Summary!G2</f>
-        <v>416.90580633024001</v>
-      </c>
-      <c r="G2">
-        <f>AVERAGE(E2:F2)</f>
-        <v>416.08316156303999</v>
-      </c>
-      <c r="H2" s="2">
-        <f t="shared" ref="H2:H14" si="0">(G2-C2)/C2</f>
-        <v>-0.29477430243552544</v>
-      </c>
-      <c r="I2" s="2">
-        <f t="shared" ref="I2:I14" si="1">(F2-G2)/C2</f>
-        <v>1.3943131647457926E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="str">
-        <f>EEZ.Summary!A3</f>
-        <v>Washington</v>
-      </c>
-      <c r="B3">
-        <f>EPRI!B3</f>
-        <v>110</v>
-      </c>
-      <c r="D3">
-        <v>172</v>
-      </c>
-      <c r="E3">
-        <f>Near.Summary!F3</f>
-        <v>68.746300301760002</v>
-      </c>
-      <c r="F3">
-        <f>Near.Summary!G3</f>
-        <v>68.991781965720008</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G8" si="2">AVERAGE(E3:F3)</f>
-        <v>68.869041133740012</v>
-      </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="str">
-        <f>EEZ.Summary!A4</f>
-        <v>Oregon</v>
-      </c>
-      <c r="B4">
-        <f>EPRI!B4</f>
-        <v>300</v>
-      </c>
-      <c r="D4">
-        <v>110</v>
-      </c>
-      <c r="E4">
-        <f>Near.Summary!F4</f>
-        <v>128.75444870051999</v>
-      </c>
-      <c r="F4">
-        <f>Near.Summary!G4</f>
-        <v>129.25055795903998</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="2"/>
-        <v>129.00250332977998</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="str">
-        <f>EEZ.Summary!A5</f>
-        <v>California</v>
-      </c>
-      <c r="B5">
-        <f>EPRI!B5</f>
-        <v>1250</v>
-      </c>
-      <c r="D5">
-        <v>803</v>
-      </c>
-      <c r="E5">
-        <f>Near.Summary!F5</f>
-        <v>218.73699725856</v>
-      </c>
-      <c r="F5">
-        <f>Near.Summary!G5</f>
-        <v>219.63841015871998</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="2"/>
-        <v>219.18770370863999</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="str">
-        <f>EEZ.Summary!A6</f>
-        <v>East Coast</v>
-      </c>
-      <c r="B6" t="str">
-        <f>EPRI!B6</f>
-        <v>N/A</v>
-      </c>
-      <c r="C6">
-        <f>EPRI!C3</f>
-        <v>240</v>
-      </c>
-      <c r="D6">
-        <v>60</v>
-      </c>
-      <c r="E6">
-        <f>Near.Summary!F6</f>
-        <v>97.745161754879987</v>
-      </c>
-      <c r="F6">
-        <f>Near.Summary!G6</f>
-        <v>93.556862546399998</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="2"/>
-        <v>95.651012150639986</v>
-      </c>
-      <c r="H6" s="2">
-        <f t="shared" si="0"/>
-        <v>-0.60145411603900001</v>
-      </c>
-      <c r="I6" s="2">
-        <f t="shared" si="1"/>
-        <v>-8.7256233509999479E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="str">
-        <f>EEZ.Summary!A7</f>
-        <v>New England</v>
-      </c>
-      <c r="B7" t="str">
-        <f>EPRI!B7</f>
-        <v>N/A</v>
-      </c>
-      <c r="E7">
-        <f>Near.Summary!F7</f>
-        <v>34.095284317439997</v>
-      </c>
-      <c r="F7">
-        <f>Near.Summary!G7</f>
-        <v>34.004854206719997</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="2"/>
-        <v>34.050069262080001</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="str">
-        <f>EEZ.Summary!A8</f>
-        <v>Mid-Atlantic</v>
-      </c>
-      <c r="D8">
-        <f>SUM(D2:D7)</f>
-        <v>1564</v>
-      </c>
-      <c r="E8">
-        <f>Near.Summary!F8</f>
-        <v>23.339961651839999</v>
-      </c>
-      <c r="F8">
-        <f>Near.Summary!G8</f>
-        <v>22.107055634879998</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="2"/>
-        <v>22.723508643359999</v>
-      </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="str">
-        <f>EEZ.Summary!A9</f>
-        <v>Southeast</v>
-      </c>
-      <c r="D9">
-        <f t="shared" ref="D9:D16" si="3">SUM(D3:D8)</f>
-        <v>2709</v>
-      </c>
-      <c r="E9">
-        <f>Near.Summary!F9</f>
-        <v>40.271730384960001</v>
-      </c>
-      <c r="F9">
-        <f>Near.Summary!G9</f>
-        <v>39.353855692800003</v>
-      </c>
-      <c r="G9">
-        <f t="shared" ref="G9:G16" si="4">AVERAGE(E9:F9)</f>
-        <v>39.812793038880002</v>
-      </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" t="str">
-        <f>EEZ.Summary!A10</f>
-        <v>Hawaii</v>
-      </c>
-      <c r="C10">
-        <f>EPRI!C4</f>
-        <v>130</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="3"/>
-        <v>5246</v>
-      </c>
-      <c r="E10">
-        <f>Near.Summary!F10</f>
-        <v>118.53569549088</v>
-      </c>
-      <c r="F10">
-        <f>Near.Summary!G10</f>
-        <v>119.15384531136</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="4"/>
-        <v>118.84477040112</v>
-      </c>
-      <c r="H10" s="2">
-        <f t="shared" si="0"/>
-        <v>-8.5809458452923065E-2</v>
-      </c>
-      <c r="I10" s="2">
-        <f t="shared" si="1"/>
-        <v>2.377499309538459E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="str">
-        <f>EEZ.Summary!A11</f>
-        <v>Alaska</v>
-      </c>
-      <c r="C11">
-        <f>EPRI!C5</f>
-        <v>1570</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="3"/>
-        <v>10382</v>
-      </c>
-      <c r="E11">
-        <f>Near.Summary!F11</f>
-        <v>1189.3491951206399</v>
-      </c>
-      <c r="F11">
-        <f>Near.Summary!G11</f>
-        <v>1194.3687709900798</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="4"/>
-        <v>1191.8589830553599</v>
-      </c>
-      <c r="H11" s="2">
-        <f t="shared" si="0"/>
-        <v>-0.24085415092015294</v>
-      </c>
-      <c r="I11" s="2">
-        <f t="shared" si="1"/>
-        <v>1.5985910412228996E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" t="str">
-        <f>EEZ.Summary!A12</f>
-        <v>Gulf of Mexico</v>
-      </c>
-      <c r="C12">
-        <f>EPRI!C6</f>
-        <v>80</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="3"/>
-        <v>19961</v>
-      </c>
-      <c r="E12">
-        <f>Near.Summary!F12</f>
-        <v>26.954782940160001</v>
-      </c>
-      <c r="F12">
-        <f>Near.Summary!G12</f>
-        <v>24.17166348816</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="4"/>
-        <v>25.563223214160001</v>
-      </c>
-      <c r="H12" s="2">
-        <f t="shared" si="0"/>
-        <v>-0.68045970982299997</v>
-      </c>
-      <c r="I12" s="2">
-        <f t="shared" si="1"/>
-        <v>-1.7394496575000008E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" t="str">
-        <f>EEZ.Summary!A13</f>
-        <v>Puerto Rico + US V.I.</v>
-      </c>
-      <c r="C13">
-        <f>EPRI!C7</f>
-        <v>30</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="3"/>
-        <v>39862</v>
-      </c>
-      <c r="E13">
-        <f>Near.Summary!F13</f>
-        <v>17.856457584000001</v>
-      </c>
-      <c r="F13">
-        <f>Near.Summary!G13</f>
-        <v>18.006283157760002</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="4"/>
-        <v>17.931370370880003</v>
-      </c>
-      <c r="H13" s="2">
-        <f t="shared" si="0"/>
-        <v>-0.40228765430399988</v>
-      </c>
-      <c r="I13" s="2">
-        <f t="shared" si="1"/>
-        <v>2.4970928959999602E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" t="str">
-        <f>EEZ.Summary!A14</f>
-        <v>Total</v>
-      </c>
-      <c r="B14">
-        <f>SUM(B2:B5)</f>
-        <v>2100</v>
-      </c>
-      <c r="C14">
-        <f>EPRI!C8</f>
-        <v>2640</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="3"/>
-        <v>79724</v>
-      </c>
-      <c r="E14">
-        <f>Near.Summary!F14</f>
-        <v>1865.7018096863999</v>
-      </c>
-      <c r="F14">
-        <f>Near.Summary!G14</f>
-        <v>1866.1632318239997</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="4"/>
-        <v>1865.9325207551997</v>
-      </c>
-      <c r="H14" s="2">
-        <f t="shared" si="0"/>
-        <v>-0.29320737850181833</v>
-      </c>
-      <c r="I14" s="2">
-        <f t="shared" si="1"/>
-        <v>8.7390556363643688E-5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Calculate bidirectional technical resource numbers.
</commit_message>
<xml_diff>
--- a/results/Total_Results.xlsx
+++ b/results/Total_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lkilcher/Dropbox/work/mhk/wave_res/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6EA1FA8-BBFE-7F4F-9B57-A83592E85894}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9CFE62-04C1-4149-A6A2-34089D563B5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33760" yWindow="460" windowWidth="28800" windowHeight="16020" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36580" yWindow="-560" windowWidth="33900" windowHeight="13160" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EEZ.bl" sheetId="2" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="70">
   <si>
     <t>bdir</t>
   </si>
@@ -264,13 +264,16 @@
     <t>Technical Ranges: nearshore - EEZ</t>
   </si>
   <si>
-    <t>Technical Ranges: near (threshold 8000 - 1000)</t>
-  </si>
-  <si>
     <t>WAVE ENERGY</t>
   </si>
   <si>
     <t>Extraction Factor (kW/m)</t>
+  </si>
+  <si>
+    <t>Technical Ranges: near (threshold 8 kW/m - 1 kW/m)</t>
+  </si>
+  <si>
+    <t>Technical (threshold: 8 KW/m)</t>
   </si>
 </sst>
 </file>
@@ -1839,8 +1842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893C187D-BAAF-1F4C-A561-9DE5DDD64B38}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1866,7 +1869,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="16">
         <f>EEZ.Summary!F$14</f>
@@ -1878,19 +1881,19 @@
       </c>
       <c r="D2" s="16">
         <f>near.technical!E14</f>
-        <v>867.40668682175999</v>
+        <v>1095.6245153971199</v>
       </c>
       <c r="E2" s="16">
         <f>EEZ.technical!E14</f>
-        <v>1040.9492832585599</v>
+        <v>2033.1433939574401</v>
       </c>
       <c r="F2" s="16">
         <f>near.technical!E15</f>
-        <v>265.87267497983999</v>
+        <v>276.99580846079999</v>
       </c>
       <c r="G2" s="16">
         <f>EEZ.technical!E15</f>
-        <v>278.02642883807999</v>
+        <v>416.53399142399996</v>
       </c>
       <c r="H2" t="s">
         <v>65</v>
@@ -1908,22 +1911,22 @@
       </c>
       <c r="D3" s="16">
         <f>near.technical!E14</f>
-        <v>867.40668682175999</v>
+        <v>1095.6245153971199</v>
       </c>
       <c r="E3" s="16">
         <f>near.technical!B14</f>
-        <v>1807.8990108662399</v>
+        <v>2111.4016100505601</v>
       </c>
       <c r="F3" s="16">
         <f>near.technical!E15</f>
-        <v>265.87267497983999</v>
+        <v>276.99580846079999</v>
       </c>
       <c r="G3" s="16">
         <f>near.technical!B15</f>
-        <v>533.96275740672002</v>
+        <v>566.43113985024002</v>
       </c>
       <c r="H3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1939,10 +1942,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F893EFA9-E3BF-F249-9404-9C034DB18919}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1951,9 +1954,10 @@
     <col min="3" max="3" width="13.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
     <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="8" max="8" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1975,8 +1979,11 @@
       <c r="G1" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="str">
         <f>EEZ.Summary!A2</f>
         <v>West Coast</v>
@@ -2005,8 +2012,12 @@
         <f>B2+E2</f>
         <v>416.90580633024001</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="13">
+        <f>near.technical!E2*0.9</f>
+        <v>249.29622761472001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="str">
         <f>EEZ.Summary!A3</f>
         <v>Washington</v>
@@ -2032,11 +2043,15 @@
         <v>68.746300301760002</v>
       </c>
       <c r="G3" s="14">
-        <f t="shared" ref="G3:G13" si="1">B3+E3</f>
+        <f t="shared" ref="G3:H13" si="1">B3+E3</f>
         <v>68.991781965720008</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="14">
+        <f>near.technical!E3*0.9</f>
+        <v>46.014311817216004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="str">
         <f>EEZ.Summary!A4</f>
         <v>Oregon</v>
@@ -2065,8 +2080,12 @@
         <f t="shared" si="1"/>
         <v>129.25055795903998</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="14">
+        <f>near.technical!E4*0.9</f>
+        <v>86.607337992192001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="str">
         <f>EEZ.Summary!A5</f>
         <v>California</v>
@@ -2095,8 +2114,12 @@
         <f t="shared" si="1"/>
         <v>219.63841015871998</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="14">
+        <f>near.technical!E5*0.9</f>
+        <v>116.67456165888001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="str">
         <f>EEZ.Summary!A6</f>
         <v>East Coast</v>
@@ -2125,8 +2148,12 @@
         <f t="shared" si="1"/>
         <v>93.556862546399998</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="13">
+        <f>near.technical!E6*0.9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="str">
         <f>EEZ.Summary!A7</f>
         <v>New England</v>
@@ -2155,8 +2182,12 @@
         <f t="shared" si="1"/>
         <v>34.004854206719997</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H7" s="14">
+        <f>near.technical!E7*0.9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="str">
         <f>EEZ.Summary!A8</f>
         <v>Mid-Atlantic</v>
@@ -2185,8 +2216,12 @@
         <f t="shared" si="1"/>
         <v>22.107055634879998</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" s="14">
+        <f>near.technical!E8*0.9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="str">
         <f>EEZ.Summary!A9</f>
         <v>Southeast</v>
@@ -2214,8 +2249,12 @@
         <f t="shared" si="1"/>
         <v>39.353855692800003</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="14">
+        <f>near.technical!E9*0.9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="str">
         <f>EEZ.Summary!A10</f>
         <v>Hawaii</v>
@@ -2244,8 +2283,12 @@
         <f t="shared" si="1"/>
         <v>119.15384531136</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" s="13">
+        <f>near.technical!E10*0.9</f>
+        <v>46.224076170240004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="str">
         <f>EEZ.Summary!A11</f>
         <v>Alaska</v>
@@ -2274,8 +2317,12 @@
         <f t="shared" si="1"/>
         <v>1194.3687709900798</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11" s="13">
+        <f>near.technical!E11*0.9</f>
+        <v>690.54176007244803</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="str">
         <f>EEZ.Summary!A12</f>
         <v>Gulf of Mexico</v>
@@ -2304,8 +2351,12 @@
         <f t="shared" si="1"/>
         <v>24.17166348816</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12" s="13">
+        <f>near.technical!E12*0.9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="str">
         <f>EEZ.Summary!A13</f>
         <v>Puerto Rico + US V.I.</v>
@@ -2334,8 +2385,12 @@
         <f t="shared" si="1"/>
         <v>18.006283157760002</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H13" s="13">
+        <f>near.technical!E13*0.9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="str">
         <f>EEZ.Summary!A14</f>
         <v>Total</v>
@@ -2363,6 +2418,10 @@
       <c r="G14" s="15">
         <f t="shared" si="2"/>
         <v>1866.1632318239997</v>
+      </c>
+      <c r="H14" s="15">
+        <f>near.technical!E14*0.9</f>
+        <v>986.06206385740791</v>
       </c>
     </row>
   </sheetData>
@@ -3644,7 +3703,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{356F04A3-FC2C-4542-8490-87ECB75F1C7E}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3672,186 +3733,186 @@
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="16">
-        <v>417.03496138752001</v>
-      </c>
-      <c r="C2" s="16">
-        <v>399.56333789183998</v>
-      </c>
-      <c r="D2" s="16">
-        <v>329.67702331392002</v>
-      </c>
-      <c r="E2" s="16">
-        <v>277.71025219583998</v>
+      <c r="B2">
+        <v>477.46797060095997</v>
+      </c>
+      <c r="C2">
+        <v>459.99638298624001</v>
+      </c>
+      <c r="D2">
+        <v>390.11003252735998</v>
+      </c>
+      <c r="E2">
+        <v>337.69519792128</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="16">
-        <v>9.6699916031999997</v>
-      </c>
-      <c r="C3" s="16">
-        <v>9.4063753113599997</v>
-      </c>
-      <c r="D3" s="16">
-        <v>8.3519073408000004</v>
-      </c>
-      <c r="E3" s="16">
-        <v>7.5610567833599998</v>
+      <c r="B3">
+        <v>10.083272985600001</v>
+      </c>
+      <c r="C3">
+        <v>9.8196566937600007</v>
+      </c>
+      <c r="D3">
+        <v>8.7651892838399998</v>
+      </c>
+      <c r="E3">
+        <v>7.9743387264000001</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="16">
-        <v>157.84685543424001</v>
-      </c>
-      <c r="C4" s="16">
-        <v>153.5264649216</v>
-      </c>
-      <c r="D4" s="16">
-        <v>136.24492978175999</v>
-      </c>
-      <c r="E4" s="16">
-        <v>123.2837941248</v>
+      <c r="B4">
+        <v>166.8283441152</v>
+      </c>
+      <c r="C4">
+        <v>162.50795360256001</v>
+      </c>
+      <c r="D4">
+        <v>145.22642743296001</v>
+      </c>
+      <c r="E4">
+        <v>132.26528280575999</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="16">
-        <v>249.51813341184001</v>
-      </c>
-      <c r="C5" s="16">
-        <v>236.63053578239999</v>
-      </c>
-      <c r="D5" s="16">
-        <v>185.08014526464001</v>
-      </c>
-      <c r="E5" s="16">
-        <v>146.86542483456</v>
+      <c r="B5">
+        <v>300.55635910656002</v>
+      </c>
+      <c r="C5">
+        <v>287.66877941759998</v>
+      </c>
+      <c r="D5">
+        <v>236.11840684032001</v>
+      </c>
+      <c r="E5">
+        <v>197.45559601151999</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="16">
-        <v>106.30601822208</v>
-      </c>
-      <c r="C6" s="16">
-        <v>89.585993195520004</v>
-      </c>
-      <c r="D6" s="16">
-        <v>24.035778263040001</v>
-      </c>
-      <c r="E6" s="16">
-        <v>0.31617664224000003</v>
+      <c r="B6">
+        <v>212.59700232192</v>
+      </c>
+      <c r="C6">
+        <v>195.87697729536001</v>
+      </c>
+      <c r="D6">
+        <v>128.99685924863999</v>
+      </c>
+      <c r="E6">
+        <v>78.838793502719994</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="16">
-        <v>26.454903982080001</v>
-      </c>
-      <c r="C7" s="16">
-        <v>22.92139413504</v>
-      </c>
-      <c r="D7" s="16">
-        <v>8.7873637171199999</v>
-      </c>
-      <c r="E7" s="16">
-        <v>2.1120219839999999E-2</v>
+      <c r="B7">
+        <v>57.971131330559999</v>
+      </c>
+      <c r="C7">
+        <v>54.437623726079998</v>
+      </c>
+      <c r="D7">
+        <v>40.303588823040002</v>
+      </c>
+      <c r="E7">
+        <v>29.703066009600001</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="16">
-        <v>20.4428069376</v>
-      </c>
-      <c r="C8" s="16">
-        <v>17.652029598719999</v>
-      </c>
-      <c r="D8" s="16">
-        <v>6.4889112729600003</v>
-      </c>
-      <c r="E8" s="16">
-        <v>0.29505642240000002</v>
+      <c r="B8">
+        <v>40.181064314879997</v>
+      </c>
+      <c r="C8">
+        <v>37.390283612159998</v>
+      </c>
+      <c r="D8">
+        <v>26.22716977152</v>
+      </c>
+      <c r="E8">
+        <v>17.854828784639999</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="16">
-        <v>59.408320757760002</v>
-      </c>
-      <c r="C9" s="16">
-        <v>49.012575068159997</v>
-      </c>
-      <c r="D9" s="16">
-        <v>8.7595060761599992</v>
-      </c>
-      <c r="E9" s="16">
-        <v>0</v>
+      <c r="B9">
+        <v>114.44481564672</v>
+      </c>
+      <c r="C9">
+        <v>104.04907892736</v>
+      </c>
+      <c r="D9">
+        <v>62.466091683839998</v>
+      </c>
+      <c r="E9">
+        <v>31.280899829759999</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="16">
-        <v>368.65472544767999</v>
-      </c>
-      <c r="C10" s="16">
-        <v>330.51132739584</v>
-      </c>
-      <c r="D10" s="16">
-        <v>191.27497506815999</v>
-      </c>
-      <c r="E10" s="16">
-        <v>109.74450855936</v>
+      <c r="B10">
+        <v>657.47481722880002</v>
+      </c>
+      <c r="C10">
+        <v>619.33149093888005</v>
+      </c>
+      <c r="D10">
+        <v>466.75797049343998</v>
+      </c>
+      <c r="E10">
+        <v>352.32784809984003</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="16">
-        <v>1041.5315075481601</v>
-      </c>
-      <c r="C11" s="16">
-        <v>992.96993820672003</v>
-      </c>
-      <c r="D11" s="16">
-        <v>798.72392097791999</v>
-      </c>
-      <c r="E11" s="16">
-        <v>653.17834586111996</v>
+      <c r="B11">
+        <v>1652.40346116096</v>
+      </c>
+      <c r="C11">
+        <v>1603.84199049216</v>
+      </c>
+      <c r="D11">
+        <v>1409.59585665024</v>
+      </c>
+      <c r="E11">
+        <v>1263.9112472985601</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="16">
-        <v>12.89082579456</v>
-      </c>
-      <c r="C12" s="16">
-        <v>4.8840075110400001</v>
-      </c>
-      <c r="D12" s="16">
-        <v>0</v>
-      </c>
-      <c r="E12" s="16">
+      <c r="B12">
+        <v>27.762354585600001</v>
+      </c>
+      <c r="C12">
+        <v>19.755536302079999</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
         <v>0</v>
       </c>
     </row>
@@ -3859,17 +3920,17 @@
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="16">
-        <v>5.8012246425600003</v>
-      </c>
-      <c r="C13" s="16">
-        <v>4.9069752499200003</v>
-      </c>
-      <c r="D13" s="16">
-        <v>1.32997767936</v>
-      </c>
-      <c r="E13" s="16">
-        <v>0</v>
+      <c r="B13">
+        <v>7.5243023462399998</v>
+      </c>
+      <c r="C13">
+        <v>6.6300529535999999</v>
+      </c>
+      <c r="D13">
+        <v>3.0530556633599999</v>
+      </c>
+      <c r="E13">
+        <v>0.37030713504000001</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -3878,19 +3939,19 @@
       </c>
       <c r="B14" s="18">
         <f>SUM(B2,B6,B10,B11,B12,B13)</f>
-        <v>1952.2192630425602</v>
+        <v>3035.2299082444797</v>
       </c>
       <c r="C14" s="18">
         <f t="shared" ref="C14:E14" si="0">SUM(C2,C6,C10,C11,C12,C13)</f>
-        <v>1822.4215794508798</v>
+        <v>2905.4324309683207</v>
       </c>
       <c r="D14" s="18">
         <f t="shared" si="0"/>
-        <v>1345.0416753023999</v>
+        <v>2398.5137745830398</v>
       </c>
       <c r="E14" s="18">
         <f t="shared" si="0"/>
-        <v>1040.9492832585599</v>
+        <v>2033.1433939574401</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -3899,19 +3960,19 @@
       </c>
       <c r="B15" s="18">
         <f>SUM(B2,B6,B12)</f>
-        <v>536.23180540416001</v>
+        <v>717.82732750847993</v>
       </c>
       <c r="C15" s="18">
         <f t="shared" ref="C15:E15" si="1">SUM(C2,C6,C12)</f>
-        <v>494.03333859840001</v>
+        <v>675.6288965836801</v>
       </c>
       <c r="D15" s="18">
         <f t="shared" si="1"/>
-        <v>353.71280157696003</v>
+        <v>519.106891776</v>
       </c>
       <c r="E15" s="18">
         <f t="shared" si="1"/>
-        <v>278.02642883807999</v>
+        <v>416.53399142399996</v>
       </c>
     </row>
   </sheetData>
@@ -5179,8 +5240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83D0FE4B-FC5C-C341-B515-8969CD7528FD}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5190,7 +5251,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -5206,184 +5267,195 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>17</v>
+      <c r="A2" t="str">
+        <f>EEZ.Summary!A2</f>
+        <v>West Coast</v>
       </c>
       <c r="B2">
-        <v>416.16007593984</v>
+        <v>438.64667357183998</v>
       </c>
       <c r="C2">
-        <v>394.43006423039998</v>
+        <v>416.25250529279998</v>
       </c>
       <c r="D2">
-        <v>316.08140464128002</v>
+        <v>331.54297675776002</v>
       </c>
       <c r="E2">
-        <v>265.87267497983999</v>
+        <v>276.99580846079999</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>44</v>
+      <c r="A3" t="str">
+        <f>EEZ.Summary!A3</f>
+        <v>Washington</v>
       </c>
       <c r="B3">
-        <v>68.940008079359998</v>
+        <v>69.208052305920006</v>
       </c>
       <c r="C3">
-        <v>66.679870894079997</v>
+        <v>66.947915120640005</v>
       </c>
       <c r="D3">
-        <v>57.639353548800003</v>
+        <v>57.907402260479998</v>
       </c>
       <c r="E3">
-        <v>50.858968903680001</v>
+        <v>51.127013130240002</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>45</v>
+      <c r="A4" t="str">
+        <f>EEZ.Summary!A4</f>
+        <v>Oregon</v>
       </c>
       <c r="B4">
-        <v>128.71922135040001</v>
+        <v>129.60620765184001</v>
       </c>
       <c r="C4">
-        <v>124.54724345856</v>
+        <v>125.43422975999999</v>
       </c>
       <c r="D4">
-        <v>107.8593318912</v>
+        <v>108.7463092224</v>
       </c>
       <c r="E4">
-        <v>95.343398215679997</v>
+        <v>96.230375546879998</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>46</v>
+      <c r="A5" t="str">
+        <f>EEZ.Summary!A5</f>
+        <v>California</v>
       </c>
       <c r="B5">
-        <v>218.50085548032001</v>
+        <v>239.83246295039999</v>
       </c>
       <c r="C5">
-        <v>203.2029364224</v>
+        <v>223.87042320384001</v>
       </c>
       <c r="D5">
-        <v>150.58271920128001</v>
+        <v>164.88928321536</v>
       </c>
       <c r="E5">
-        <v>119.67030337536001</v>
+        <v>129.6384018432</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>12</v>
+      <c r="A6" t="str">
+        <f>EEZ.Summary!A6</f>
+        <v>East Coast</v>
       </c>
       <c r="B6">
-        <v>93.279884206079998</v>
+        <v>100.72070725632</v>
       </c>
       <c r="C6">
-        <v>65.337541754879993</v>
+        <v>72.757298196479994</v>
       </c>
       <c r="D6">
-        <v>2.5341160665600002</v>
+        <v>5.4632742144000002</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>47</v>
+      <c r="A7" t="str">
+        <f>EEZ.Summary!A7</f>
+        <v>New England</v>
       </c>
       <c r="B7">
-        <v>31.332826306560001</v>
+        <v>35.611702548479997</v>
       </c>
       <c r="C7">
-        <v>24.279127418880002</v>
+        <v>28.558005903360002</v>
       </c>
       <c r="D7">
-        <v>1.2534424704</v>
+        <v>3.1959129023999999</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>48</v>
+      <c r="A8" t="str">
+        <f>EEZ.Summary!A8</f>
+        <v>Mid-Atlantic</v>
       </c>
       <c r="B8">
-        <v>22.466746490879999</v>
+        <v>23.697683189759999</v>
       </c>
       <c r="C8">
-        <v>16.63279953408</v>
+        <v>17.863739596799999</v>
       </c>
       <c r="D8">
-        <v>0.39242914847999999</v>
+        <v>0.81326865887999999</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>49</v>
+      <c r="A9" t="str">
+        <f>EEZ.Summary!A9</f>
+        <v>Southeast</v>
       </c>
       <c r="B9">
-        <v>39.480309166079998</v>
+        <v>41.41131927552</v>
       </c>
       <c r="C9">
-        <v>24.425611438080001</v>
+        <v>26.335557181439999</v>
       </c>
       <c r="D9">
-        <v>0.88824437759999997</v>
+        <v>1.4540924428799999</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>14</v>
+      <c r="A10" t="str">
+        <f>EEZ.Summary!A10</f>
+        <v>Hawaii</v>
       </c>
       <c r="B10">
-        <v>118.27432323072</v>
+        <v>156.26498276352001</v>
       </c>
       <c r="C10">
-        <v>102.9542252544</v>
+        <v>140.9357127168</v>
       </c>
       <c r="D10">
-        <v>54.840301163520003</v>
+        <v>83.536595650560002</v>
       </c>
       <c r="E10">
-        <v>31.03552676352</v>
+        <v>51.360084633600003</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>11</v>
+      <c r="A11" t="str">
+        <f>EEZ.Summary!A11</f>
+        <v>Alaska</v>
       </c>
       <c r="B11">
-        <v>1137.97040634528</v>
+        <v>1368.7883937484801</v>
       </c>
       <c r="C11">
-        <v>1045.82996603424</v>
+        <v>1274.5286279260799</v>
       </c>
       <c r="D11">
-        <v>752.99074399487995</v>
+        <v>966.68525630208001</v>
       </c>
       <c r="E11">
-        <v>570.49848507839999</v>
+        <v>767.26862230272002</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>13</v>
+      <c r="A12" t="str">
+        <f>EEZ.Summary!A12</f>
+        <v>Gulf of Mexico</v>
       </c>
       <c r="B12">
-        <v>24.522797260800001</v>
+        <v>27.063759022079999</v>
       </c>
       <c r="C12">
-        <v>8.3624669952000001</v>
+        <v>9.5402236262399995</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -5393,17 +5465,18 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>15</v>
+      <c r="A13" t="str">
+        <f>EEZ.Summary!A13</f>
+        <v>Puerto Rico + US V.I.</v>
       </c>
       <c r="B13">
-        <v>17.691523883519999</v>
+        <v>19.917093688320001</v>
       </c>
       <c r="C13">
-        <v>12.68265287424</v>
+        <v>14.342561587200001</v>
       </c>
       <c r="D13">
-        <v>2.1331920307200001</v>
+        <v>2.2932756345600001</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -5415,19 +5488,19 @@
       </c>
       <c r="B14" s="1">
         <f>SUM(B2,B6,B10:B13)</f>
-        <v>1807.8990108662399</v>
+        <v>2111.4016100505601</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" ref="C14:E14" si="0">SUM(C2,C6,C10:C13)</f>
-        <v>1629.5969171433599</v>
+        <v>1928.3569293455998</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
-        <v>1128.57975789696</v>
+        <v>1389.5213785593598</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>867.40668682175999</v>
+        <v>1095.6245153971199</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -5436,19 +5509,19 @@
       </c>
       <c r="B15" s="1">
         <f>SUM(B2,B6,B12)</f>
-        <v>533.96275740672002</v>
+        <v>566.43113985024002</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" ref="C15:E15" si="1">SUM(C2,C6,C12)</f>
-        <v>468.13007298047995</v>
+        <v>498.55002711551998</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="1"/>
-        <v>318.61552070784001</v>
+        <v>337.00625097215999</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="1"/>
-        <v>265.87267497983999</v>
+        <v>276.99580846079999</v>
       </c>
     </row>
   </sheetData>
@@ -5556,10 +5629,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5570,9 +5643,10 @@
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
     <col min="5" max="5" width="15.5" customWidth="1"/>
     <col min="6" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -5594,8 +5668,11 @@
       <c r="G1" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -5623,8 +5700,12 @@
         <f>B2+E2</f>
         <v>623.06666299392009</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="13">
+        <f>EEZ.technical!E2*0.9</f>
+        <v>303.925678129152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>50</v>
       </c>
@@ -5652,8 +5733,12 @@
         <f t="shared" ref="G3:G7" si="1">B3+E3</f>
         <v>25.354693954559998</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="14">
+        <f>EEZ.technical!E3*0.9</f>
+        <v>7.17690485376</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>51</v>
       </c>
@@ -5681,8 +5766,12 @@
         <f t="shared" si="1"/>
         <v>208.02196912127999</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="14">
+        <f>EEZ.technical!E4*0.9</f>
+        <v>119.038754525184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>52</v>
       </c>
@@ -5710,8 +5799,12 @@
         <f t="shared" si="1"/>
         <v>390.31777431552001</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="14">
+        <f>EEZ.technical!E5*0.9</f>
+        <v>177.71003641036799</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
@@ -5739,8 +5832,12 @@
         <f t="shared" si="1"/>
         <v>341.05888542720004</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="13">
+        <f>EEZ.technical!E6*0.9</f>
+        <v>70.954914152447998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>53</v>
       </c>
@@ -5768,8 +5865,12 @@
         <f t="shared" si="1"/>
         <v>105.28089470975999</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H7" s="14">
+        <f>EEZ.technical!E7*0.9</f>
+        <v>26.73275940864</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>54</v>
       </c>
@@ -5797,8 +5898,12 @@
         <f t="shared" ref="G8:G13" si="3">B8+E8</f>
         <v>75.999683389439994</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" s="14">
+        <f>EEZ.technical!E8*0.9</f>
+        <v>16.069345906176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>55</v>
       </c>
@@ -5826,8 +5931,12 @@
         <f t="shared" si="3"/>
         <v>159.0242353152</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="14">
+        <f>EEZ.technical!E9*0.9</f>
+        <v>28.152809846783999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>24</v>
       </c>
@@ -5855,8 +5964,12 @@
         <f t="shared" si="3"/>
         <v>471.6069144576</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" s="13">
+        <f>EEZ.technical!E10*0.9</f>
+        <v>317.09506328985606</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
@@ -5884,8 +5997,12 @@
         <f t="shared" si="3"/>
         <v>2551.0858791321598</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11" s="13">
+        <f>EEZ.technical!E11*0.9</f>
+        <v>1137.520122568704</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
@@ -5913,8 +6030,12 @@
         <f t="shared" si="3"/>
         <v>69.647607521279994</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12" s="13">
+        <f>EEZ.technical!E12*0.9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
@@ -5942,8 +6063,12 @@
         <f t="shared" si="3"/>
         <v>32.719640547840001</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H13" s="13">
+        <f>EEZ.technical!E13*0.9</f>
+        <v>0.33327642153600001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>56</v>
       </c>
@@ -5970,6 +6095,10 @@
       <c r="G14" s="15">
         <f t="shared" si="4"/>
         <v>4089.1855900799997</v>
+      </c>
+      <c r="H14" s="15">
+        <f>EEZ.technical!E14*0.9</f>
+        <v>1829.8290545616962</v>
       </c>
     </row>
   </sheetData>

</xml_diff>